<commit_message>
forcewave 20230501 언제 다하냐
</commit_message>
<xml_diff>
--- a/document/일정표_최경수.xlsx
+++ b/document/일정표_최경수.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\facci\Desktop\Dukkeobi\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48A3F23-4257-407B-B27F-2F36574D2CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797DC66F-082E-4084-9E88-EFF0349C97DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-2810" windowWidth="25820" windowHeight="15500" xr2:uid="{4F68EF3D-DEC7-4864-A746-04C7E98A59CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4F68EF3D-DEC7-4864-A746-04C7E98A59CC}"/>
   </bookViews>
   <sheets>
     <sheet name="일정표" sheetId="1" r:id="rId1"/>
@@ -1082,7 +1082,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1332,6 +1332,12 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1485,7 +1491,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1810,29 +1816,29 @@
   <dimension ref="A1:BT84"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R40" sqref="R40"/>
+      <pane ySplit="8" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V47" sqref="V47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="19.899999999999999" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="19.899999999999999" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="5.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.125" style="4" customWidth="1"/>
-    <col min="7" max="8" width="3.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.08203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.08203125" style="4" customWidth="1"/>
+    <col min="7" max="8" width="3.08203125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="1.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="28" width="1.875" style="4" customWidth="1"/>
-    <col min="29" max="30" width="1.875" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="28" width="1.83203125" style="4" customWidth="1"/>
+    <col min="29" max="30" width="1.83203125" style="4" hidden="1" customWidth="1"/>
     <col min="31" max="70" width="8.75" style="1" hidden="1" customWidth="1"/>
     <col min="71" max="72" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="73" max="16384" width="8.75" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1847,30 +1853,30 @@
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="1"/>
-      <c r="J2" s="100" t="s">
+      <c r="J2" s="102" t="s">
         <v>122</v>
       </c>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="N2" s="86" t="s">
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="N2" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="O2" s="87"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="87"/>
-      <c r="R2" s="87"/>
-      <c r="S2" s="87"/>
-      <c r="T2" s="87"/>
-      <c r="U2" s="87"/>
-      <c r="V2" s="87"/>
-      <c r="W2" s="87"/>
-      <c r="X2" s="87"/>
-      <c r="Y2" s="87"/>
-      <c r="Z2" s="87"/>
-      <c r="AA2" s="87"/>
-      <c r="AB2" s="88"/>
-    </row>
-    <row r="3" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O2" s="89"/>
+      <c r="P2" s="89"/>
+      <c r="Q2" s="89"/>
+      <c r="R2" s="89"/>
+      <c r="S2" s="89"/>
+      <c r="T2" s="89"/>
+      <c r="U2" s="89"/>
+      <c r="V2" s="89"/>
+      <c r="W2" s="89"/>
+      <c r="X2" s="89"/>
+      <c r="Y2" s="89"/>
+      <c r="Z2" s="89"/>
+      <c r="AA2" s="89"/>
+      <c r="AB2" s="90"/>
+    </row>
+    <row r="3" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1885,28 +1891,28 @@
       </c>
       <c r="F3" s="71"/>
       <c r="G3" s="73"/>
-      <c r="J3" s="101" t="s">
+      <c r="J3" s="103" t="s">
         <v>121</v>
       </c>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
-      <c r="Q3" s="90"/>
-      <c r="R3" s="90"/>
-      <c r="S3" s="90"/>
-      <c r="T3" s="90"/>
-      <c r="U3" s="90"/>
-      <c r="V3" s="90"/>
-      <c r="W3" s="90"/>
-      <c r="X3" s="90"/>
-      <c r="Y3" s="90"/>
-      <c r="Z3" s="90"/>
-      <c r="AA3" s="90"/>
-      <c r="AB3" s="91"/>
-    </row>
-    <row r="4" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="103"/>
+      <c r="L3" s="103"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="92"/>
+      <c r="P3" s="92"/>
+      <c r="Q3" s="92"/>
+      <c r="R3" s="92"/>
+      <c r="S3" s="92"/>
+      <c r="T3" s="92"/>
+      <c r="U3" s="92"/>
+      <c r="V3" s="92"/>
+      <c r="W3" s="92"/>
+      <c r="X3" s="92"/>
+      <c r="Y3" s="92"/>
+      <c r="Z3" s="92"/>
+      <c r="AA3" s="92"/>
+      <c r="AB3" s="93"/>
+    </row>
+    <row r="4" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1921,132 +1927,132 @@
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="1"/>
-      <c r="J4" s="102" t="s">
+      <c r="J4" s="104" t="s">
         <v>132</v>
       </c>
-      <c r="K4" s="102"/>
-      <c r="L4" s="102"/>
-      <c r="N4" s="92"/>
-      <c r="O4" s="93"/>
-      <c r="P4" s="93"/>
-      <c r="Q4" s="93"/>
-      <c r="R4" s="93"/>
-      <c r="S4" s="93"/>
-      <c r="T4" s="93"/>
-      <c r="U4" s="93"/>
-      <c r="V4" s="93"/>
-      <c r="W4" s="93"/>
-      <c r="X4" s="93"/>
-      <c r="Y4" s="93"/>
-      <c r="Z4" s="93"/>
-      <c r="AA4" s="93"/>
-      <c r="AB4" s="94"/>
-    </row>
-    <row r="5" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K4" s="104"/>
+      <c r="L4" s="104"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="95"/>
+      <c r="Q4" s="95"/>
+      <c r="R4" s="95"/>
+      <c r="S4" s="95"/>
+      <c r="T4" s="95"/>
+      <c r="U4" s="95"/>
+      <c r="V4" s="95"/>
+      <c r="W4" s="95"/>
+      <c r="X4" s="95"/>
+      <c r="Y4" s="95"/>
+      <c r="Z4" s="95"/>
+      <c r="AA4" s="95"/>
+      <c r="AB4" s="96"/>
+    </row>
+    <row r="5" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:30" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="114" t="s">
+    <row r="6" spans="1:30" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="116" t="s">
         <v>152</v>
       </c>
-      <c r="C6" s="103" t="s">
+      <c r="C6" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="103" t="s">
+      <c r="D6" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="103" t="s">
+      <c r="E6" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="103" t="s">
+      <c r="F6" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="103" t="s">
+      <c r="G6" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="95" t="s">
+      <c r="H6" s="97" t="s">
         <v>151</v>
       </c>
       <c r="I6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="97" t="s">
+      <c r="J6" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="97"/>
-      <c r="L6" s="97"/>
-      <c r="M6" s="97"/>
-      <c r="N6" s="97"/>
-      <c r="O6" s="97"/>
-      <c r="P6" s="97"/>
-      <c r="Q6" s="97"/>
-      <c r="R6" s="97"/>
-      <c r="S6" s="97"/>
-      <c r="T6" s="97"/>
-      <c r="U6" s="97"/>
-      <c r="V6" s="97"/>
-      <c r="W6" s="98"/>
-      <c r="X6" s="99" t="s">
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="99"/>
+      <c r="N6" s="99"/>
+      <c r="O6" s="99"/>
+      <c r="P6" s="99"/>
+      <c r="Q6" s="99"/>
+      <c r="R6" s="99"/>
+      <c r="S6" s="99"/>
+      <c r="T6" s="99"/>
+      <c r="U6" s="99"/>
+      <c r="V6" s="99"/>
+      <c r="W6" s="100"/>
+      <c r="X6" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="Y6" s="97"/>
-      <c r="Z6" s="97"/>
-      <c r="AA6" s="97"/>
-      <c r="AB6" s="97"/>
-      <c r="AC6" s="97"/>
-      <c r="AD6" s="98"/>
-    </row>
-    <row r="7" spans="1:30" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y6" s="99"/>
+      <c r="Z6" s="99"/>
+      <c r="AA6" s="99"/>
+      <c r="AB6" s="99"/>
+      <c r="AC6" s="99"/>
+      <c r="AD6" s="100"/>
+    </row>
+    <row r="7" spans="1:30" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
-      <c r="B7" s="115"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="103"/>
-      <c r="G7" s="103"/>
-      <c r="H7" s="96"/>
+      <c r="B7" s="117"/>
+      <c r="C7" s="105"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="105"/>
+      <c r="H7" s="98"/>
       <c r="I7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="84" t="s">
+      <c r="J7" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="84"/>
-      <c r="L7" s="84"/>
-      <c r="M7" s="84"/>
-      <c r="N7" s="84"/>
-      <c r="O7" s="84"/>
-      <c r="P7" s="84"/>
-      <c r="Q7" s="83" t="s">
+      <c r="K7" s="86"/>
+      <c r="L7" s="86"/>
+      <c r="M7" s="86"/>
+      <c r="N7" s="86"/>
+      <c r="O7" s="86"/>
+      <c r="P7" s="86"/>
+      <c r="Q7" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="84"/>
-      <c r="S7" s="84"/>
-      <c r="T7" s="84"/>
-      <c r="U7" s="84"/>
-      <c r="V7" s="84"/>
-      <c r="W7" s="84"/>
-      <c r="X7" s="83" t="s">
+      <c r="R7" s="86"/>
+      <c r="S7" s="86"/>
+      <c r="T7" s="86"/>
+      <c r="U7" s="86"/>
+      <c r="V7" s="86"/>
+      <c r="W7" s="86"/>
+      <c r="X7" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="Y7" s="84"/>
-      <c r="Z7" s="84"/>
-      <c r="AA7" s="84"/>
-      <c r="AB7" s="84"/>
-      <c r="AC7" s="84"/>
-      <c r="AD7" s="85"/>
-    </row>
-    <row r="8" spans="1:30" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y7" s="86"/>
+      <c r="Z7" s="86"/>
+      <c r="AA7" s="86"/>
+      <c r="AB7" s="86"/>
+      <c r="AC7" s="86"/>
+      <c r="AD7" s="87"/>
+    </row>
+    <row r="8" spans="1:30" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
-      <c r="B8" s="116"/>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="103"/>
-      <c r="F8" s="103"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="96"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="105"/>
+      <c r="G8" s="105"/>
+      <c r="H8" s="98"/>
       <c r="I8" s="13" t="s">
         <v>13</v>
       </c>
@@ -2114,11 +2120,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="117" t="s">
+    <row r="9" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="111" t="s">
+      <c r="C9" s="113" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="14" t="s">
@@ -2155,15 +2161,15 @@
       <c r="Y9" s="14"/>
       <c r="Z9" s="14"/>
       <c r="AA9" s="14"/>
-      <c r="AB9" s="122" t="s">
+      <c r="AB9" s="124" t="s">
         <v>133</v>
       </c>
       <c r="AC9" s="53"/>
       <c r="AD9" s="54"/>
     </row>
-    <row r="10" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="107"/>
-      <c r="C10" s="112"/>
+    <row r="10" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="109"/>
+      <c r="C10" s="114"/>
       <c r="D10" s="18" t="s">
         <v>81</v>
       </c>
@@ -2198,13 +2204,13 @@
       <c r="Y10" s="18"/>
       <c r="Z10" s="18"/>
       <c r="AA10" s="18"/>
-      <c r="AB10" s="123"/>
+      <c r="AB10" s="125"/>
       <c r="AC10" s="55"/>
       <c r="AD10" s="56"/>
     </row>
-    <row r="11" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="107"/>
-      <c r="C11" s="113"/>
+    <row r="11" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="109"/>
+      <c r="C11" s="115"/>
       <c r="D11" s="22" t="s">
         <v>82</v>
       </c>
@@ -2239,16 +2245,16 @@
       <c r="Y11" s="22"/>
       <c r="Z11" s="22"/>
       <c r="AA11" s="22"/>
-      <c r="AB11" s="123"/>
+      <c r="AB11" s="125"/>
       <c r="AC11" s="57"/>
       <c r="AD11" s="58"/>
     </row>
-    <row r="12" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="107"/>
-      <c r="C12" s="111" t="s">
+    <row r="12" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="109"/>
+      <c r="C12" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="121" t="s">
+      <c r="D12" s="123" t="s">
         <v>83</v>
       </c>
       <c r="E12" s="14" t="s">
@@ -2280,14 +2286,14 @@
       <c r="Y12" s="14"/>
       <c r="Z12" s="14"/>
       <c r="AA12" s="14"/>
-      <c r="AB12" s="123"/>
+      <c r="AB12" s="125"/>
       <c r="AC12" s="53"/>
       <c r="AD12" s="54"/>
     </row>
-    <row r="13" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="107"/>
-      <c r="C13" s="112"/>
-      <c r="D13" s="109"/>
+    <row r="13" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B13" s="109"/>
+      <c r="C13" s="114"/>
+      <c r="D13" s="111"/>
       <c r="E13" s="18" t="s">
         <v>64</v>
       </c>
@@ -2317,14 +2323,14 @@
       <c r="Y13" s="18"/>
       <c r="Z13" s="18"/>
       <c r="AA13" s="18"/>
-      <c r="AB13" s="123"/>
+      <c r="AB13" s="125"/>
       <c r="AC13" s="55"/>
       <c r="AD13" s="56"/>
     </row>
-    <row r="14" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="107"/>
-      <c r="C14" s="112"/>
-      <c r="D14" s="109"/>
+    <row r="14" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="109"/>
+      <c r="C14" s="114"/>
+      <c r="D14" s="111"/>
       <c r="E14" s="18" t="s">
         <v>65</v>
       </c>
@@ -2354,14 +2360,14 @@
       <c r="Y14" s="18"/>
       <c r="Z14" s="18"/>
       <c r="AA14" s="18"/>
-      <c r="AB14" s="123"/>
+      <c r="AB14" s="125"/>
       <c r="AC14" s="55"/>
       <c r="AD14" s="56"/>
     </row>
-    <row r="15" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="107"/>
-      <c r="C15" s="112"/>
-      <c r="D15" s="109"/>
+    <row r="15" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="109"/>
+      <c r="C15" s="114"/>
+      <c r="D15" s="111"/>
       <c r="E15" s="18" t="s">
         <v>72</v>
       </c>
@@ -2391,14 +2397,14 @@
       <c r="Y15" s="18"/>
       <c r="Z15" s="18"/>
       <c r="AA15" s="18"/>
-      <c r="AB15" s="123"/>
+      <c r="AB15" s="125"/>
       <c r="AC15" s="55"/>
       <c r="AD15" s="56"/>
     </row>
-    <row r="16" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="107"/>
-      <c r="C16" s="112"/>
-      <c r="D16" s="109"/>
+    <row r="16" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="109"/>
+      <c r="C16" s="114"/>
+      <c r="D16" s="111"/>
       <c r="E16" s="18" t="s">
         <v>66</v>
       </c>
@@ -2428,14 +2434,14 @@
       <c r="Y16" s="18"/>
       <c r="Z16" s="18"/>
       <c r="AA16" s="18"/>
-      <c r="AB16" s="123"/>
+      <c r="AB16" s="125"/>
       <c r="AC16" s="55"/>
       <c r="AD16" s="56"/>
     </row>
-    <row r="17" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="107"/>
-      <c r="C17" s="112"/>
-      <c r="D17" s="109"/>
+    <row r="17" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="109"/>
+      <c r="C17" s="114"/>
+      <c r="D17" s="111"/>
       <c r="E17" s="18" t="s">
         <v>67</v>
       </c>
@@ -2465,14 +2471,14 @@
       <c r="Y17" s="18"/>
       <c r="Z17" s="18"/>
       <c r="AA17" s="18"/>
-      <c r="AB17" s="123"/>
+      <c r="AB17" s="125"/>
       <c r="AC17" s="55"/>
       <c r="AD17" s="56"/>
     </row>
-    <row r="18" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="107"/>
-      <c r="C18" s="112"/>
-      <c r="D18" s="109"/>
+    <row r="18" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="109"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="111"/>
       <c r="E18" s="18" t="s">
         <v>68</v>
       </c>
@@ -2502,14 +2508,14 @@
       <c r="Y18" s="18"/>
       <c r="Z18" s="18"/>
       <c r="AA18" s="18"/>
-      <c r="AB18" s="123"/>
+      <c r="AB18" s="125"/>
       <c r="AC18" s="55"/>
       <c r="AD18" s="56"/>
     </row>
-    <row r="19" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="107"/>
-      <c r="C19" s="112"/>
-      <c r="D19" s="109"/>
+    <row r="19" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="109"/>
+      <c r="C19" s="114"/>
+      <c r="D19" s="111"/>
       <c r="E19" s="18" t="s">
         <v>69</v>
       </c>
@@ -2539,14 +2545,14 @@
       <c r="Y19" s="18"/>
       <c r="Z19" s="18"/>
       <c r="AA19" s="18"/>
-      <c r="AB19" s="123"/>
+      <c r="AB19" s="125"/>
       <c r="AC19" s="55"/>
       <c r="AD19" s="56"/>
     </row>
-    <row r="20" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="107"/>
-      <c r="C20" s="113"/>
-      <c r="D20" s="110"/>
+    <row r="20" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="109"/>
+      <c r="C20" s="115"/>
+      <c r="D20" s="112"/>
       <c r="E20" s="22" t="s">
         <v>70</v>
       </c>
@@ -2576,12 +2582,12 @@
       <c r="Y20" s="22"/>
       <c r="Z20" s="22"/>
       <c r="AA20" s="22"/>
-      <c r="AB20" s="123"/>
+      <c r="AB20" s="125"/>
       <c r="AC20" s="57"/>
       <c r="AD20" s="58"/>
     </row>
-    <row r="21" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="107"/>
+    <row r="21" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="109"/>
       <c r="C21" s="36" t="s">
         <v>59</v>
       </c>
@@ -2619,12 +2625,12 @@
       <c r="Y21" s="18"/>
       <c r="Z21" s="18"/>
       <c r="AA21" s="18"/>
-      <c r="AB21" s="123"/>
+      <c r="AB21" s="125"/>
       <c r="AC21" s="55"/>
       <c r="AD21" s="56"/>
     </row>
-    <row r="22" spans="2:30" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="108"/>
+    <row r="22" spans="2:30" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B22" s="110"/>
       <c r="C22" s="68" t="s">
         <v>135</v>
       </c>
@@ -2662,18 +2668,18 @@
       <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
       <c r="AA22" s="42"/>
-      <c r="AB22" s="123"/>
+      <c r="AB22" s="125"/>
       <c r="AC22" s="59"/>
       <c r="AD22" s="60"/>
     </row>
-    <row r="23" spans="2:30" ht="19.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="107" t="s">
+    <row r="23" spans="2:30" ht="19.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="109" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="118" t="s">
+      <c r="C23" s="120" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="120" t="s">
+      <c r="D23" s="122" t="s">
         <v>73</v>
       </c>
       <c r="E23" s="30" t="s">
@@ -2707,14 +2713,14 @@
       <c r="Y23" s="30"/>
       <c r="Z23" s="30"/>
       <c r="AA23" s="30"/>
-      <c r="AB23" s="123"/>
+      <c r="AB23" s="125"/>
       <c r="AC23" s="61"/>
       <c r="AD23" s="62"/>
     </row>
-    <row r="24" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="107"/>
-      <c r="C24" s="119"/>
-      <c r="D24" s="109"/>
+    <row r="24" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="109"/>
+      <c r="C24" s="121"/>
+      <c r="D24" s="111"/>
       <c r="E24" s="18" t="s">
         <v>75</v>
       </c>
@@ -2746,14 +2752,14 @@
       <c r="Y24" s="18"/>
       <c r="Z24" s="18"/>
       <c r="AA24" s="18"/>
-      <c r="AB24" s="123"/>
+      <c r="AB24" s="125"/>
       <c r="AC24" s="55"/>
       <c r="AD24" s="56"/>
     </row>
-    <row r="25" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="107"/>
-      <c r="C25" s="119"/>
-      <c r="D25" s="109"/>
+    <row r="25" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="109"/>
+      <c r="C25" s="121"/>
+      <c r="D25" s="111"/>
       <c r="E25" s="18" t="s">
         <v>141</v>
       </c>
@@ -2785,12 +2791,12 @@
       <c r="Y25" s="18"/>
       <c r="Z25" s="18"/>
       <c r="AA25" s="18"/>
-      <c r="AB25" s="123"/>
+      <c r="AB25" s="125"/>
       <c r="AC25" s="55"/>
       <c r="AD25" s="56"/>
     </row>
-    <row r="26" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="107"/>
+    <row r="26" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B26" s="109"/>
       <c r="C26" s="38" t="s">
         <v>54</v>
       </c>
@@ -2828,12 +2834,12 @@
       <c r="Y26" s="18"/>
       <c r="Z26" s="18"/>
       <c r="AA26" s="18"/>
-      <c r="AB26" s="123"/>
+      <c r="AB26" s="125"/>
       <c r="AC26" s="55"/>
       <c r="AD26" s="56"/>
     </row>
-    <row r="27" spans="2:30" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="108"/>
+    <row r="27" spans="2:30" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B27" s="110"/>
       <c r="C27" s="37" t="s">
         <v>55</v>
       </c>
@@ -2871,12 +2877,12 @@
       <c r="Y27" s="26"/>
       <c r="Z27" s="26"/>
       <c r="AA27" s="26"/>
-      <c r="AB27" s="123"/>
+      <c r="AB27" s="125"/>
       <c r="AC27" s="59"/>
       <c r="AD27" s="60"/>
     </row>
-    <row r="28" spans="2:30" ht="19.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="106" t="s">
+    <row r="28" spans="2:30" ht="19.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="108" t="s">
         <v>123</v>
       </c>
       <c r="C28" s="38" t="s">
@@ -2915,12 +2921,12 @@
       <c r="Y28" s="18"/>
       <c r="Z28" s="18"/>
       <c r="AA28" s="18"/>
-      <c r="AB28" s="123"/>
+      <c r="AB28" s="125"/>
       <c r="AC28" s="55"/>
       <c r="AD28" s="55"/>
     </row>
-    <row r="29" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="107"/>
+    <row r="29" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="109"/>
       <c r="C29" s="38" t="s">
         <v>125</v>
       </c>
@@ -2957,12 +2963,12 @@
       <c r="Y29" s="18"/>
       <c r="Z29" s="18"/>
       <c r="AA29" s="18"/>
-      <c r="AB29" s="123"/>
+      <c r="AB29" s="125"/>
       <c r="AC29" s="55"/>
       <c r="AD29" s="55"/>
     </row>
-    <row r="30" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="107"/>
+    <row r="30" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="109"/>
       <c r="C30" s="38" t="s">
         <v>126</v>
       </c>
@@ -2999,12 +3005,12 @@
       <c r="Y30" s="18"/>
       <c r="Z30" s="18"/>
       <c r="AA30" s="18"/>
-      <c r="AB30" s="123"/>
+      <c r="AB30" s="125"/>
       <c r="AC30" s="55"/>
       <c r="AD30" s="55"/>
     </row>
-    <row r="31" spans="2:30" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="108"/>
+    <row r="31" spans="2:30" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B31" s="110"/>
       <c r="C31" s="37" t="s">
         <v>83</v>
       </c>
@@ -3042,21 +3048,21 @@
       <c r="Y31" s="26"/>
       <c r="Z31" s="26"/>
       <c r="AA31" s="26"/>
-      <c r="AB31" s="123"/>
+      <c r="AB31" s="125"/>
       <c r="AC31" s="59"/>
       <c r="AD31" s="59"/>
     </row>
-    <row r="32" spans="2:30" ht="19.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="104" t="s">
+    <row r="32" spans="2:30" ht="19.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="106" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="112" t="s">
+      <c r="C32" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="125" t="s">
+      <c r="D32" s="127" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="125"/>
+      <c r="E32" s="127"/>
       <c r="F32" s="19" t="s">
         <v>14</v>
       </c>
@@ -3073,25 +3079,25 @@
       <c r="M32" s="19"/>
       <c r="N32" s="47"/>
       <c r="Q32" s="19"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
-      <c r="T32" s="19"/>
+      <c r="R32" s="83"/>
+      <c r="S32" s="83"/>
+      <c r="T32" s="83"/>
       <c r="U32" s="50"/>
       <c r="V32" s="19"/>
       <c r="W32" s="19"/>
       <c r="X32" s="19"/>
       <c r="Y32" s="19"/>
-      <c r="Z32" s="128" t="s">
+      <c r="Z32" s="130" t="s">
         <v>134</v>
       </c>
-      <c r="AA32" s="129"/>
-      <c r="AB32" s="123"/>
+      <c r="AA32" s="131"/>
+      <c r="AB32" s="125"/>
       <c r="AC32" s="63"/>
       <c r="AD32" s="64"/>
     </row>
-    <row r="33" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="104"/>
-      <c r="C33" s="112"/>
+    <row r="33" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B33" s="106"/>
+      <c r="C33" s="114"/>
       <c r="D33" s="18" t="s">
         <v>24</v>
       </c>
@@ -3114,7 +3120,7 @@
       <c r="M33" s="19"/>
       <c r="N33" s="47"/>
       <c r="Q33" s="19"/>
-      <c r="R33" s="134"/>
+      <c r="R33" s="83"/>
       <c r="S33" s="19"/>
       <c r="T33" s="19"/>
       <c r="U33" s="50"/>
@@ -3122,15 +3128,15 @@
       <c r="W33" s="19"/>
       <c r="X33" s="19"/>
       <c r="Y33" s="19"/>
-      <c r="Z33" s="130"/>
-      <c r="AA33" s="131"/>
-      <c r="AB33" s="123"/>
+      <c r="Z33" s="132"/>
+      <c r="AA33" s="133"/>
+      <c r="AB33" s="125"/>
       <c r="AC33" s="63"/>
       <c r="AD33" s="64"/>
     </row>
-    <row r="34" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="104"/>
-      <c r="C34" s="112"/>
+    <row r="34" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B34" s="106"/>
+      <c r="C34" s="114"/>
       <c r="D34" s="18" t="s">
         <v>23</v>
       </c>
@@ -3153,23 +3159,23 @@
       <c r="M34" s="19"/>
       <c r="N34" s="47"/>
       <c r="Q34" s="19"/>
-      <c r="R34" s="19"/>
-      <c r="S34" s="19"/>
-      <c r="T34" s="19"/>
+      <c r="R34" s="83"/>
+      <c r="S34" s="83"/>
+      <c r="T34" s="83"/>
       <c r="U34" s="50"/>
       <c r="V34" s="19"/>
       <c r="W34" s="19"/>
       <c r="X34" s="19"/>
       <c r="Y34" s="19"/>
-      <c r="Z34" s="130"/>
-      <c r="AA34" s="131"/>
-      <c r="AB34" s="123"/>
+      <c r="Z34" s="132"/>
+      <c r="AA34" s="133"/>
+      <c r="AB34" s="125"/>
       <c r="AC34" s="63"/>
       <c r="AD34" s="64"/>
     </row>
-    <row r="35" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="104"/>
-      <c r="C35" s="112"/>
+    <row r="35" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B35" s="106"/>
+      <c r="C35" s="114"/>
       <c r="D35" s="18" t="s">
         <v>26</v>
       </c>
@@ -3193,23 +3199,23 @@
       <c r="N35" s="47"/>
       <c r="Q35" s="19"/>
       <c r="R35" s="19"/>
-      <c r="S35" s="19"/>
+      <c r="S35" s="83"/>
       <c r="T35" s="19"/>
       <c r="U35" s="50"/>
       <c r="V35" s="19"/>
       <c r="W35" s="19"/>
       <c r="X35" s="19"/>
       <c r="Y35" s="19"/>
-      <c r="Z35" s="130"/>
-      <c r="AA35" s="131"/>
-      <c r="AB35" s="123"/>
+      <c r="Z35" s="132"/>
+      <c r="AA35" s="133"/>
+      <c r="AB35" s="125"/>
       <c r="AC35" s="63"/>
       <c r="AD35" s="64"/>
     </row>
-    <row r="36" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="104"/>
-      <c r="C36" s="112"/>
-      <c r="D36" s="109" t="s">
+    <row r="36" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B36" s="106"/>
+      <c r="C36" s="114"/>
+      <c r="D36" s="111" t="s">
         <v>28</v>
       </c>
       <c r="E36" s="18" t="s">
@@ -3239,16 +3245,16 @@
       <c r="W36" s="19"/>
       <c r="X36" s="19"/>
       <c r="Y36" s="19"/>
-      <c r="Z36" s="130"/>
-      <c r="AA36" s="131"/>
-      <c r="AB36" s="123"/>
+      <c r="Z36" s="132"/>
+      <c r="AA36" s="133"/>
+      <c r="AB36" s="125"/>
       <c r="AC36" s="63"/>
       <c r="AD36" s="64"/>
     </row>
-    <row r="37" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="104"/>
-      <c r="C37" s="112"/>
-      <c r="D37" s="109"/>
+    <row r="37" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B37" s="106"/>
+      <c r="C37" s="114"/>
+      <c r="D37" s="111"/>
       <c r="E37" s="18" t="s">
         <v>30</v>
       </c>
@@ -3276,16 +3282,16 @@
       <c r="W37" s="19"/>
       <c r="X37" s="19"/>
       <c r="Y37" s="19"/>
-      <c r="Z37" s="130"/>
-      <c r="AA37" s="131"/>
-      <c r="AB37" s="123"/>
+      <c r="Z37" s="132"/>
+      <c r="AA37" s="133"/>
+      <c r="AB37" s="125"/>
       <c r="AC37" s="63"/>
       <c r="AD37" s="64"/>
     </row>
-    <row r="38" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="104"/>
-      <c r="C38" s="113"/>
-      <c r="D38" s="110"/>
+    <row r="38" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B38" s="106"/>
+      <c r="C38" s="115"/>
+      <c r="D38" s="112"/>
       <c r="E38" s="22" t="s">
         <v>31</v>
       </c>
@@ -3313,21 +3319,21 @@
       <c r="W38" s="23"/>
       <c r="X38" s="23"/>
       <c r="Y38" s="23"/>
-      <c r="Z38" s="130"/>
-      <c r="AA38" s="131"/>
-      <c r="AB38" s="123"/>
+      <c r="Z38" s="132"/>
+      <c r="AA38" s="133"/>
+      <c r="AB38" s="125"/>
       <c r="AC38" s="65"/>
       <c r="AD38" s="66"/>
     </row>
-    <row r="39" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="104"/>
-      <c r="C39" s="111" t="s">
+    <row r="39" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B39" s="106"/>
+      <c r="C39" s="113" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="126" t="s">
+      <c r="D39" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="E39" s="126"/>
+      <c r="E39" s="128"/>
       <c r="F39" s="15" t="s">
         <v>14</v>
       </c>
@@ -3347,22 +3353,22 @@
       <c r="P39" s="49"/>
       <c r="Q39" s="11"/>
       <c r="R39" s="15"/>
-      <c r="S39" s="11"/>
+      <c r="S39" s="136"/>
       <c r="T39" s="15"/>
       <c r="U39" s="51"/>
       <c r="V39" s="15"/>
       <c r="W39" s="15"/>
       <c r="X39" s="15"/>
       <c r="Y39" s="31"/>
-      <c r="Z39" s="130"/>
-      <c r="AA39" s="131"/>
-      <c r="AB39" s="123"/>
+      <c r="Z39" s="132"/>
+      <c r="AA39" s="133"/>
+      <c r="AB39" s="125"/>
       <c r="AC39" s="63"/>
       <c r="AD39" s="63"/>
     </row>
-    <row r="40" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="104"/>
-      <c r="C40" s="112"/>
+    <row r="40" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B40" s="106"/>
+      <c r="C40" s="114"/>
       <c r="D40" s="18" t="s">
         <v>35</v>
       </c>
@@ -3387,21 +3393,22 @@
       <c r="O40" s="47"/>
       <c r="P40" s="19"/>
       <c r="R40" s="19"/>
+      <c r="S40" s="84"/>
       <c r="T40" s="19"/>
       <c r="U40" s="50"/>
       <c r="V40" s="19"/>
       <c r="W40" s="19"/>
       <c r="X40" s="19"/>
       <c r="Y40" s="32"/>
-      <c r="Z40" s="130"/>
-      <c r="AA40" s="131"/>
-      <c r="AB40" s="123"/>
+      <c r="Z40" s="132"/>
+      <c r="AA40" s="133"/>
+      <c r="AB40" s="125"/>
       <c r="AC40" s="63"/>
       <c r="AD40" s="63"/>
     </row>
-    <row r="41" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="104"/>
-      <c r="C41" s="112"/>
+    <row r="41" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="106"/>
+      <c r="C41" s="114"/>
       <c r="D41" s="18" t="s">
         <v>36</v>
       </c>
@@ -3426,21 +3433,22 @@
       <c r="O41" s="47"/>
       <c r="P41" s="47"/>
       <c r="R41" s="19"/>
+      <c r="S41" s="84"/>
       <c r="T41" s="19"/>
       <c r="U41" s="50"/>
       <c r="V41" s="19"/>
       <c r="W41" s="19"/>
       <c r="X41" s="19"/>
       <c r="Y41" s="32"/>
-      <c r="Z41" s="130"/>
-      <c r="AA41" s="131"/>
-      <c r="AB41" s="123"/>
+      <c r="Z41" s="132"/>
+      <c r="AA41" s="133"/>
+      <c r="AB41" s="125"/>
       <c r="AC41" s="63"/>
       <c r="AD41" s="63"/>
     </row>
-    <row r="42" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="104"/>
-      <c r="C42" s="112"/>
+    <row r="42" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B42" s="106"/>
+      <c r="C42" s="114"/>
       <c r="D42" s="18" t="s">
         <v>39</v>
       </c>
@@ -3465,22 +3473,23 @@
       <c r="O42" s="47"/>
       <c r="P42" s="19"/>
       <c r="R42" s="19"/>
+      <c r="S42" s="84"/>
       <c r="T42" s="19"/>
       <c r="U42" s="50"/>
       <c r="V42" s="19"/>
       <c r="W42" s="19"/>
       <c r="X42" s="19"/>
       <c r="Y42" s="32"/>
-      <c r="Z42" s="130"/>
-      <c r="AA42" s="131"/>
-      <c r="AB42" s="123"/>
+      <c r="Z42" s="132"/>
+      <c r="AA42" s="133"/>
+      <c r="AB42" s="125"/>
       <c r="AC42" s="63"/>
       <c r="AD42" s="63"/>
     </row>
-    <row r="43" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="104"/>
-      <c r="C43" s="112"/>
-      <c r="D43" s="109" t="s">
+    <row r="43" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B43" s="106"/>
+      <c r="C43" s="114"/>
+      <c r="D43" s="111" t="s">
         <v>41</v>
       </c>
       <c r="E43" s="18" t="s">
@@ -3509,16 +3518,16 @@
       <c r="W43" s="19"/>
       <c r="X43" s="19"/>
       <c r="Y43" s="32"/>
-      <c r="Z43" s="130"/>
-      <c r="AA43" s="131"/>
-      <c r="AB43" s="123"/>
+      <c r="Z43" s="132"/>
+      <c r="AA43" s="133"/>
+      <c r="AB43" s="125"/>
       <c r="AC43" s="63"/>
       <c r="AD43" s="63"/>
     </row>
-    <row r="44" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="104"/>
-      <c r="C44" s="113"/>
-      <c r="D44" s="110"/>
+    <row r="44" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B44" s="106"/>
+      <c r="C44" s="115"/>
+      <c r="D44" s="112"/>
       <c r="E44" s="22" t="s">
         <v>43</v>
       </c>
@@ -3546,21 +3555,21 @@
       <c r="W44" s="23"/>
       <c r="X44" s="23"/>
       <c r="Y44" s="33"/>
-      <c r="Z44" s="130"/>
-      <c r="AA44" s="131"/>
-      <c r="AB44" s="123"/>
+      <c r="Z44" s="132"/>
+      <c r="AA44" s="133"/>
+      <c r="AB44" s="125"/>
       <c r="AC44" s="65"/>
       <c r="AD44" s="65"/>
     </row>
-    <row r="45" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="104"/>
-      <c r="C45" s="111" t="s">
+    <row r="45" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B45" s="106"/>
+      <c r="C45" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="D45" s="127" t="s">
+      <c r="D45" s="129" t="s">
         <v>146</v>
       </c>
-      <c r="E45" s="127"/>
+      <c r="E45" s="129"/>
       <c r="F45" s="15" t="s">
         <v>14</v>
       </c>
@@ -3580,23 +3589,23 @@
       <c r="P45" s="49"/>
       <c r="Q45" s="11"/>
       <c r="R45" s="15"/>
-      <c r="S45" s="11"/>
-      <c r="T45" s="11"/>
+      <c r="S45" s="136"/>
+      <c r="T45" s="136"/>
       <c r="U45" s="15"/>
       <c r="V45" s="51"/>
       <c r="W45" s="15"/>
       <c r="X45" s="15"/>
       <c r="Y45" s="31"/>
-      <c r="Z45" s="130"/>
-      <c r="AA45" s="131"/>
-      <c r="AB45" s="123"/>
+      <c r="Z45" s="132"/>
+      <c r="AA45" s="133"/>
+      <c r="AB45" s="125"/>
       <c r="AC45" s="63"/>
       <c r="AD45" s="63"/>
     </row>
-    <row r="46" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="104"/>
-      <c r="C46" s="112"/>
-      <c r="D46" s="109" t="s">
+    <row r="46" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B46" s="106"/>
+      <c r="C46" s="114"/>
+      <c r="D46" s="111" t="s">
         <v>45</v>
       </c>
       <c r="E46" s="18" t="s">
@@ -3620,21 +3629,22 @@
       <c r="O46" s="19"/>
       <c r="P46" s="47"/>
       <c r="R46" s="19"/>
+      <c r="T46" s="84"/>
       <c r="U46" s="19"/>
       <c r="V46" s="50"/>
       <c r="W46" s="19"/>
       <c r="X46" s="19"/>
       <c r="Y46" s="32"/>
-      <c r="Z46" s="130"/>
-      <c r="AA46" s="131"/>
-      <c r="AB46" s="123"/>
+      <c r="Z46" s="132"/>
+      <c r="AA46" s="133"/>
+      <c r="AB46" s="125"/>
       <c r="AC46" s="63"/>
       <c r="AD46" s="63"/>
     </row>
-    <row r="47" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="104"/>
-      <c r="C47" s="112"/>
-      <c r="D47" s="109"/>
+    <row r="47" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B47" s="106"/>
+      <c r="C47" s="114"/>
+      <c r="D47" s="111"/>
       <c r="E47" s="18" t="s">
         <v>47</v>
       </c>
@@ -3656,21 +3666,22 @@
       <c r="O47" s="19"/>
       <c r="P47" s="47"/>
       <c r="R47" s="19"/>
+      <c r="T47" s="84"/>
       <c r="U47" s="19"/>
       <c r="V47" s="50"/>
       <c r="W47" s="19"/>
       <c r="X47" s="19"/>
       <c r="Y47" s="32"/>
-      <c r="Z47" s="130"/>
-      <c r="AA47" s="131"/>
-      <c r="AB47" s="123"/>
+      <c r="Z47" s="132"/>
+      <c r="AA47" s="133"/>
+      <c r="AB47" s="125"/>
       <c r="AC47" s="63"/>
       <c r="AD47" s="63"/>
     </row>
-    <row r="48" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="104"/>
-      <c r="C48" s="112"/>
-      <c r="D48" s="109"/>
+    <row r="48" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B48" s="106"/>
+      <c r="C48" s="114"/>
+      <c r="D48" s="111"/>
       <c r="E48" s="18" t="s">
         <v>48</v>
       </c>
@@ -3692,21 +3703,22 @@
       <c r="O48" s="19"/>
       <c r="P48" s="47"/>
       <c r="R48" s="19"/>
+      <c r="T48" s="84"/>
       <c r="U48" s="19"/>
       <c r="V48" s="50"/>
       <c r="W48" s="19"/>
       <c r="X48" s="19"/>
       <c r="Y48" s="32"/>
-      <c r="Z48" s="130"/>
-      <c r="AA48" s="131"/>
-      <c r="AB48" s="123"/>
+      <c r="Z48" s="132"/>
+      <c r="AA48" s="133"/>
+      <c r="AB48" s="125"/>
       <c r="AC48" s="63"/>
       <c r="AD48" s="63"/>
     </row>
-    <row r="49" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="104"/>
-      <c r="C49" s="112"/>
-      <c r="D49" s="109"/>
+    <row r="49" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B49" s="106"/>
+      <c r="C49" s="114"/>
+      <c r="D49" s="111"/>
       <c r="E49" s="18" t="s">
         <v>131</v>
       </c>
@@ -3728,20 +3740,21 @@
       <c r="O49" s="19"/>
       <c r="P49" s="47"/>
       <c r="R49" s="19"/>
+      <c r="T49" s="84"/>
       <c r="U49" s="19"/>
       <c r="V49" s="50"/>
       <c r="W49" s="19"/>
       <c r="X49" s="19"/>
       <c r="Y49" s="32"/>
-      <c r="Z49" s="130"/>
-      <c r="AA49" s="131"/>
-      <c r="AB49" s="123"/>
+      <c r="Z49" s="132"/>
+      <c r="AA49" s="133"/>
+      <c r="AB49" s="125"/>
       <c r="AC49" s="63"/>
       <c r="AD49" s="63"/>
     </row>
-    <row r="50" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="104"/>
-      <c r="C50" s="113"/>
+    <row r="50" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B50" s="106"/>
+      <c r="C50" s="115"/>
       <c r="D50" s="22" t="s">
         <v>49</v>
       </c>
@@ -3772,22 +3785,22 @@
       <c r="W50" s="23"/>
       <c r="X50" s="23"/>
       <c r="Y50" s="33"/>
-      <c r="Z50" s="130"/>
-      <c r="AA50" s="131"/>
-      <c r="AB50" s="123"/>
+      <c r="Z50" s="132"/>
+      <c r="AA50" s="133"/>
+      <c r="AB50" s="125"/>
       <c r="AC50" s="63"/>
       <c r="AD50" s="63"/>
     </row>
-    <row r="51" spans="1:30" s="10" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:30" s="10" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="1"/>
-      <c r="B51" s="104"/>
-      <c r="C51" s="111" t="s">
+      <c r="B51" s="106"/>
+      <c r="C51" s="113" t="s">
         <v>84</v>
       </c>
-      <c r="D51" s="127" t="s">
+      <c r="D51" s="129" t="s">
         <v>91</v>
       </c>
-      <c r="E51" s="127"/>
+      <c r="E51" s="129"/>
       <c r="F51" s="19" t="s">
         <v>14</v>
       </c>
@@ -3811,16 +3824,16 @@
       <c r="W51" s="15"/>
       <c r="X51" s="15"/>
       <c r="Y51" s="15"/>
-      <c r="Z51" s="130"/>
-      <c r="AA51" s="131"/>
-      <c r="AB51" s="123"/>
+      <c r="Z51" s="132"/>
+      <c r="AA51" s="133"/>
+      <c r="AB51" s="125"/>
       <c r="AC51" s="67"/>
       <c r="AD51" s="67"/>
     </row>
-    <row r="52" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="104"/>
-      <c r="C52" s="112"/>
-      <c r="D52" s="109" t="s">
+    <row r="52" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="106"/>
+      <c r="C52" s="114"/>
+      <c r="D52" s="111" t="s">
         <v>85</v>
       </c>
       <c r="E52" s="18" t="s">
@@ -3849,16 +3862,16 @@
       <c r="W52" s="19"/>
       <c r="X52" s="19"/>
       <c r="Y52" s="19"/>
-      <c r="Z52" s="130"/>
-      <c r="AA52" s="131"/>
-      <c r="AB52" s="123"/>
+      <c r="Z52" s="132"/>
+      <c r="AA52" s="133"/>
+      <c r="AB52" s="125"/>
       <c r="AC52" s="63"/>
       <c r="AD52" s="63"/>
     </row>
-    <row r="53" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="104"/>
-      <c r="C53" s="112"/>
-      <c r="D53" s="109"/>
+    <row r="53" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="106"/>
+      <c r="C53" s="114"/>
+      <c r="D53" s="111"/>
       <c r="E53" s="18" t="s">
         <v>87</v>
       </c>
@@ -3885,16 +3898,16 @@
       <c r="W53" s="19"/>
       <c r="X53" s="19"/>
       <c r="Y53" s="19"/>
-      <c r="Z53" s="130"/>
-      <c r="AA53" s="131"/>
-      <c r="AB53" s="123"/>
+      <c r="Z53" s="132"/>
+      <c r="AA53" s="133"/>
+      <c r="AB53" s="125"/>
       <c r="AC53" s="63"/>
       <c r="AD53" s="63"/>
     </row>
-    <row r="54" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="104"/>
-      <c r="C54" s="112"/>
-      <c r="D54" s="109"/>
+    <row r="54" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B54" s="106"/>
+      <c r="C54" s="114"/>
+      <c r="D54" s="111"/>
       <c r="E54" s="18" t="s">
         <v>88</v>
       </c>
@@ -3921,17 +3934,17 @@
       <c r="W54" s="19"/>
       <c r="X54" s="19"/>
       <c r="Y54" s="19"/>
-      <c r="Z54" s="130"/>
-      <c r="AA54" s="131"/>
-      <c r="AB54" s="123"/>
+      <c r="Z54" s="132"/>
+      <c r="AA54" s="133"/>
+      <c r="AB54" s="125"/>
       <c r="AC54" s="63"/>
       <c r="AD54" s="63"/>
     </row>
-    <row r="55" spans="1:30" s="6" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:30" s="6" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="1"/>
-      <c r="B55" s="104"/>
-      <c r="C55" s="113"/>
-      <c r="D55" s="110"/>
+      <c r="B55" s="106"/>
+      <c r="C55" s="115"/>
+      <c r="D55" s="112"/>
       <c r="E55" s="22" t="s">
         <v>89</v>
       </c>
@@ -3958,22 +3971,22 @@
       <c r="W55" s="23"/>
       <c r="X55" s="23"/>
       <c r="Y55" s="23"/>
-      <c r="Z55" s="130"/>
-      <c r="AA55" s="131"/>
-      <c r="AB55" s="123"/>
+      <c r="Z55" s="132"/>
+      <c r="AA55" s="133"/>
+      <c r="AB55" s="125"/>
       <c r="AC55" s="65"/>
       <c r="AD55" s="65"/>
     </row>
-    <row r="56" spans="1:30" s="10" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:30" s="10" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="1"/>
-      <c r="B56" s="104"/>
-      <c r="C56" s="111" t="s">
+      <c r="B56" s="106"/>
+      <c r="C56" s="113" t="s">
         <v>90</v>
       </c>
-      <c r="D56" s="127" t="s">
+      <c r="D56" s="129" t="s">
         <v>92</v>
       </c>
-      <c r="E56" s="127"/>
+      <c r="E56" s="129"/>
       <c r="F56" s="19" t="s">
         <v>14</v>
       </c>
@@ -4000,16 +4013,16 @@
       <c r="W56" s="51"/>
       <c r="X56" s="51"/>
       <c r="Y56" s="15"/>
-      <c r="Z56" s="130"/>
-      <c r="AA56" s="131"/>
-      <c r="AB56" s="123"/>
+      <c r="Z56" s="132"/>
+      <c r="AA56" s="133"/>
+      <c r="AB56" s="125"/>
       <c r="AC56" s="67"/>
       <c r="AD56" s="67"/>
     </row>
-    <row r="57" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="104"/>
-      <c r="C57" s="112"/>
-      <c r="D57" s="109" t="s">
+    <row r="57" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B57" s="106"/>
+      <c r="C57" s="114"/>
+      <c r="D57" s="111" t="s">
         <v>93</v>
       </c>
       <c r="E57" s="18" t="s">
@@ -4041,16 +4054,16 @@
       <c r="W57" s="50"/>
       <c r="X57" s="50"/>
       <c r="Y57" s="19"/>
-      <c r="Z57" s="130"/>
-      <c r="AA57" s="131"/>
-      <c r="AB57" s="123"/>
+      <c r="Z57" s="132"/>
+      <c r="AA57" s="133"/>
+      <c r="AB57" s="125"/>
       <c r="AC57" s="63"/>
       <c r="AD57" s="63"/>
     </row>
-    <row r="58" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="104"/>
-      <c r="C58" s="112"/>
-      <c r="D58" s="109"/>
+    <row r="58" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B58" s="106"/>
+      <c r="C58" s="114"/>
+      <c r="D58" s="111"/>
       <c r="E58" s="18" t="s">
         <v>95</v>
       </c>
@@ -4080,16 +4093,16 @@
       <c r="W58" s="50"/>
       <c r="X58" s="50"/>
       <c r="Y58" s="19"/>
-      <c r="Z58" s="130"/>
-      <c r="AA58" s="131"/>
-      <c r="AB58" s="123"/>
+      <c r="Z58" s="132"/>
+      <c r="AA58" s="133"/>
+      <c r="AB58" s="125"/>
       <c r="AC58" s="63"/>
       <c r="AD58" s="63"/>
     </row>
-    <row r="59" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="104"/>
-      <c r="C59" s="112"/>
-      <c r="D59" s="109"/>
+    <row r="59" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B59" s="106"/>
+      <c r="C59" s="114"/>
+      <c r="D59" s="111"/>
       <c r="E59" s="18" t="s">
         <v>96</v>
       </c>
@@ -4119,16 +4132,16 @@
       <c r="W59" s="50"/>
       <c r="X59" s="50"/>
       <c r="Y59" s="19"/>
-      <c r="Z59" s="130"/>
-      <c r="AA59" s="131"/>
-      <c r="AB59" s="123"/>
+      <c r="Z59" s="132"/>
+      <c r="AA59" s="133"/>
+      <c r="AB59" s="125"/>
       <c r="AC59" s="63"/>
       <c r="AD59" s="63"/>
     </row>
-    <row r="60" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="104"/>
-      <c r="C60" s="112"/>
-      <c r="D60" s="109"/>
+    <row r="60" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B60" s="106"/>
+      <c r="C60" s="114"/>
+      <c r="D60" s="111"/>
       <c r="E60" s="18" t="s">
         <v>97</v>
       </c>
@@ -4158,16 +4171,16 @@
       <c r="W60" s="50"/>
       <c r="X60" s="50"/>
       <c r="Y60" s="19"/>
-      <c r="Z60" s="130"/>
-      <c r="AA60" s="131"/>
-      <c r="AB60" s="123"/>
+      <c r="Z60" s="132"/>
+      <c r="AA60" s="133"/>
+      <c r="AB60" s="125"/>
       <c r="AC60" s="63"/>
       <c r="AD60" s="63"/>
     </row>
-    <row r="61" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="104"/>
-      <c r="C61" s="112"/>
-      <c r="D61" s="109" t="s">
+    <row r="61" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B61" s="106"/>
+      <c r="C61" s="114"/>
+      <c r="D61" s="111" t="s">
         <v>98</v>
       </c>
       <c r="E61" s="18" t="s">
@@ -4197,16 +4210,16 @@
       <c r="W61" s="19"/>
       <c r="X61" s="19"/>
       <c r="Y61" s="19"/>
-      <c r="Z61" s="130"/>
-      <c r="AA61" s="131"/>
-      <c r="AB61" s="123"/>
+      <c r="Z61" s="132"/>
+      <c r="AA61" s="133"/>
+      <c r="AB61" s="125"/>
       <c r="AC61" s="63"/>
       <c r="AD61" s="63"/>
     </row>
-    <row r="62" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="104"/>
-      <c r="C62" s="112"/>
-      <c r="D62" s="109"/>
+    <row r="62" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B62" s="106"/>
+      <c r="C62" s="114"/>
+      <c r="D62" s="111"/>
       <c r="E62" s="18" t="s">
         <v>100</v>
       </c>
@@ -4234,17 +4247,17 @@
       <c r="W62" s="19"/>
       <c r="X62" s="19"/>
       <c r="Y62" s="19"/>
-      <c r="Z62" s="130"/>
-      <c r="AA62" s="131"/>
-      <c r="AB62" s="123"/>
+      <c r="Z62" s="132"/>
+      <c r="AA62" s="133"/>
+      <c r="AB62" s="125"/>
       <c r="AC62" s="63"/>
       <c r="AD62" s="63"/>
     </row>
-    <row r="63" spans="1:30" s="6" customFormat="1" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:30" s="6" customFormat="1" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="1"/>
-      <c r="B63" s="104"/>
-      <c r="C63" s="113"/>
-      <c r="D63" s="110"/>
+      <c r="B63" s="106"/>
+      <c r="C63" s="115"/>
+      <c r="D63" s="112"/>
       <c r="E63" s="22" t="s">
         <v>101</v>
       </c>
@@ -4272,22 +4285,22 @@
       <c r="W63" s="23"/>
       <c r="X63" s="23"/>
       <c r="Y63" s="23"/>
-      <c r="Z63" s="130"/>
-      <c r="AA63" s="131"/>
-      <c r="AB63" s="123"/>
+      <c r="Z63" s="132"/>
+      <c r="AA63" s="133"/>
+      <c r="AB63" s="125"/>
       <c r="AC63" s="65"/>
       <c r="AD63" s="65"/>
     </row>
-    <row r="64" spans="1:30" s="10" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:30" s="10" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="1"/>
-      <c r="B64" s="104"/>
-      <c r="C64" s="111" t="s">
+      <c r="B64" s="106"/>
+      <c r="C64" s="113" t="s">
         <v>102</v>
       </c>
-      <c r="D64" s="127" t="s">
+      <c r="D64" s="129" t="s">
         <v>103</v>
       </c>
-      <c r="E64" s="127"/>
+      <c r="E64" s="129"/>
       <c r="F64" s="15" t="s">
         <v>14</v>
       </c>
@@ -4314,16 +4327,16 @@
       <c r="W64" s="15"/>
       <c r="X64" s="51"/>
       <c r="Y64" s="15"/>
-      <c r="Z64" s="130"/>
-      <c r="AA64" s="131"/>
-      <c r="AB64" s="123"/>
+      <c r="Z64" s="132"/>
+      <c r="AA64" s="133"/>
+      <c r="AB64" s="125"/>
       <c r="AC64" s="67"/>
       <c r="AD64" s="67"/>
     </row>
-    <row r="65" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="104"/>
-      <c r="C65" s="112"/>
-      <c r="D65" s="109" t="s">
+    <row r="65" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B65" s="106"/>
+      <c r="C65" s="114"/>
+      <c r="D65" s="111" t="s">
         <v>104</v>
       </c>
       <c r="E65" s="18" t="s">
@@ -4355,16 +4368,16 @@
       <c r="W65" s="19"/>
       <c r="X65" s="50"/>
       <c r="Y65" s="19"/>
-      <c r="Z65" s="130"/>
-      <c r="AA65" s="131"/>
-      <c r="AB65" s="123"/>
+      <c r="Z65" s="132"/>
+      <c r="AA65" s="133"/>
+      <c r="AB65" s="125"/>
       <c r="AC65" s="63"/>
       <c r="AD65" s="63"/>
     </row>
-    <row r="66" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="104"/>
-      <c r="C66" s="112"/>
-      <c r="D66" s="109"/>
+    <row r="66" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B66" s="106"/>
+      <c r="C66" s="114"/>
+      <c r="D66" s="111"/>
       <c r="E66" s="18" t="s">
         <v>106</v>
       </c>
@@ -4394,16 +4407,16 @@
       <c r="W66" s="19"/>
       <c r="X66" s="50"/>
       <c r="Y66" s="19"/>
-      <c r="Z66" s="130"/>
-      <c r="AA66" s="131"/>
-      <c r="AB66" s="123"/>
+      <c r="Z66" s="132"/>
+      <c r="AA66" s="133"/>
+      <c r="AB66" s="125"/>
       <c r="AC66" s="63"/>
       <c r="AD66" s="63"/>
     </row>
-    <row r="67" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="104"/>
-      <c r="C67" s="112"/>
-      <c r="D67" s="109"/>
+    <row r="67" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B67" s="106"/>
+      <c r="C67" s="114"/>
+      <c r="D67" s="111"/>
       <c r="E67" s="18" t="s">
         <v>107</v>
       </c>
@@ -4433,16 +4446,16 @@
       <c r="W67" s="19"/>
       <c r="X67" s="50"/>
       <c r="Y67" s="19"/>
-      <c r="Z67" s="130"/>
-      <c r="AA67" s="131"/>
-      <c r="AB67" s="123"/>
+      <c r="Z67" s="132"/>
+      <c r="AA67" s="133"/>
+      <c r="AB67" s="125"/>
       <c r="AC67" s="63"/>
       <c r="AD67" s="63"/>
     </row>
-    <row r="68" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="104"/>
-      <c r="C68" s="112"/>
-      <c r="D68" s="109"/>
+    <row r="68" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B68" s="106"/>
+      <c r="C68" s="114"/>
+      <c r="D68" s="111"/>
       <c r="E68" s="18" t="s">
         <v>108</v>
       </c>
@@ -4472,16 +4485,16 @@
       <c r="W68" s="19"/>
       <c r="X68" s="50"/>
       <c r="Y68" s="19"/>
-      <c r="Z68" s="130"/>
-      <c r="AA68" s="131"/>
-      <c r="AB68" s="123"/>
+      <c r="Z68" s="132"/>
+      <c r="AA68" s="133"/>
+      <c r="AB68" s="125"/>
       <c r="AC68" s="63"/>
       <c r="AD68" s="63"/>
     </row>
-    <row r="69" spans="1:30" s="6" customFormat="1" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:30" s="6" customFormat="1" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="1"/>
-      <c r="B69" s="104"/>
-      <c r="C69" s="113"/>
+      <c r="B69" s="106"/>
+      <c r="C69" s="115"/>
       <c r="D69" s="22" t="s">
         <v>109</v>
       </c>
@@ -4512,21 +4525,21 @@
       <c r="W69" s="23"/>
       <c r="X69" s="23"/>
       <c r="Y69" s="23"/>
-      <c r="Z69" s="130"/>
-      <c r="AA69" s="131"/>
-      <c r="AB69" s="123"/>
+      <c r="Z69" s="132"/>
+      <c r="AA69" s="133"/>
+      <c r="AB69" s="125"/>
       <c r="AC69" s="65"/>
       <c r="AD69" s="65"/>
     </row>
-    <row r="70" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="104"/>
-      <c r="C70" s="111" t="s">
+    <row r="70" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B70" s="106"/>
+      <c r="C70" s="113" t="s">
         <v>147</v>
       </c>
-      <c r="D70" s="126" t="s">
+      <c r="D70" s="128" t="s">
         <v>111</v>
       </c>
-      <c r="E70" s="126"/>
+      <c r="E70" s="128"/>
       <c r="F70" s="15" t="s">
         <v>14</v>
       </c>
@@ -4553,16 +4566,16 @@
       <c r="W70" s="15"/>
       <c r="X70" s="15"/>
       <c r="Y70" s="74"/>
-      <c r="Z70" s="130"/>
-      <c r="AA70" s="131"/>
-      <c r="AB70" s="123"/>
+      <c r="Z70" s="132"/>
+      <c r="AA70" s="133"/>
+      <c r="AB70" s="125"/>
       <c r="AC70" s="63"/>
       <c r="AD70" s="63"/>
     </row>
-    <row r="71" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="104"/>
-      <c r="C71" s="112"/>
-      <c r="D71" s="109" t="s">
+    <row r="71" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B71" s="106"/>
+      <c r="C71" s="114"/>
+      <c r="D71" s="111" t="s">
         <v>112</v>
       </c>
       <c r="E71" s="18" t="s">
@@ -4594,16 +4607,16 @@
       <c r="W71" s="19"/>
       <c r="X71" s="19"/>
       <c r="Y71" s="75"/>
-      <c r="Z71" s="130"/>
-      <c r="AA71" s="131"/>
-      <c r="AB71" s="123"/>
+      <c r="Z71" s="132"/>
+      <c r="AA71" s="133"/>
+      <c r="AB71" s="125"/>
       <c r="AC71" s="63"/>
       <c r="AD71" s="63"/>
     </row>
-    <row r="72" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="104"/>
-      <c r="C72" s="112"/>
-      <c r="D72" s="109"/>
+    <row r="72" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B72" s="106"/>
+      <c r="C72" s="114"/>
+      <c r="D72" s="111"/>
       <c r="E72" s="18" t="s">
         <v>114</v>
       </c>
@@ -4633,16 +4646,16 @@
       <c r="W72" s="19"/>
       <c r="X72" s="19"/>
       <c r="Y72" s="75"/>
-      <c r="Z72" s="130"/>
-      <c r="AA72" s="131"/>
-      <c r="AB72" s="123"/>
+      <c r="Z72" s="132"/>
+      <c r="AA72" s="133"/>
+      <c r="AB72" s="125"/>
       <c r="AC72" s="63"/>
       <c r="AD72" s="63"/>
     </row>
-    <row r="73" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="104"/>
-      <c r="C73" s="112"/>
-      <c r="D73" s="109"/>
+    <row r="73" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B73" s="106"/>
+      <c r="C73" s="114"/>
+      <c r="D73" s="111"/>
       <c r="E73" s="18" t="s">
         <v>115</v>
       </c>
@@ -4672,16 +4685,16 @@
       <c r="W73" s="19"/>
       <c r="X73" s="19"/>
       <c r="Y73" s="75"/>
-      <c r="Z73" s="130"/>
-      <c r="AA73" s="131"/>
-      <c r="AB73" s="123"/>
+      <c r="Z73" s="132"/>
+      <c r="AA73" s="133"/>
+      <c r="AB73" s="125"/>
       <c r="AC73" s="63"/>
       <c r="AD73" s="63"/>
     </row>
-    <row r="74" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="104"/>
-      <c r="C74" s="112"/>
-      <c r="D74" s="109" t="s">
+    <row r="74" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B74" s="106"/>
+      <c r="C74" s="114"/>
+      <c r="D74" s="111" t="s">
         <v>116</v>
       </c>
       <c r="E74" s="18" t="s">
@@ -4713,16 +4726,16 @@
       <c r="W74" s="19"/>
       <c r="X74" s="19"/>
       <c r="Y74" s="75"/>
-      <c r="Z74" s="130"/>
-      <c r="AA74" s="131"/>
-      <c r="AB74" s="123"/>
+      <c r="Z74" s="132"/>
+      <c r="AA74" s="133"/>
+      <c r="AB74" s="125"/>
       <c r="AC74" s="63"/>
       <c r="AD74" s="63"/>
     </row>
-    <row r="75" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="104"/>
-      <c r="C75" s="112"/>
-      <c r="D75" s="109"/>
+    <row r="75" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B75" s="106"/>
+      <c r="C75" s="114"/>
+      <c r="D75" s="111"/>
       <c r="E75" s="18" t="s">
         <v>118</v>
       </c>
@@ -4752,16 +4765,16 @@
       <c r="W75" s="19"/>
       <c r="X75" s="19"/>
       <c r="Y75" s="75"/>
-      <c r="Z75" s="130"/>
-      <c r="AA75" s="131"/>
-      <c r="AB75" s="123"/>
+      <c r="Z75" s="132"/>
+      <c r="AA75" s="133"/>
+      <c r="AB75" s="125"/>
       <c r="AC75" s="63"/>
       <c r="AD75" s="63"/>
     </row>
-    <row r="76" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="104"/>
-      <c r="C76" s="112"/>
-      <c r="D76" s="109"/>
+    <row r="76" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B76" s="106"/>
+      <c r="C76" s="114"/>
+      <c r="D76" s="111"/>
       <c r="E76" s="18" t="s">
         <v>119</v>
       </c>
@@ -4791,17 +4804,17 @@
       <c r="W76" s="19"/>
       <c r="X76" s="19"/>
       <c r="Y76" s="75"/>
-      <c r="Z76" s="130"/>
-      <c r="AA76" s="131"/>
-      <c r="AB76" s="123"/>
+      <c r="Z76" s="132"/>
+      <c r="AA76" s="133"/>
+      <c r="AB76" s="125"/>
       <c r="AC76" s="63"/>
       <c r="AD76" s="63"/>
     </row>
-    <row r="77" spans="1:30" s="6" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:30" s="6" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="1"/>
-      <c r="B77" s="105"/>
-      <c r="C77" s="113"/>
-      <c r="D77" s="110"/>
+      <c r="B77" s="107"/>
+      <c r="C77" s="115"/>
+      <c r="D77" s="112"/>
       <c r="E77" s="22" t="s">
         <v>120</v>
       </c>
@@ -4831,21 +4844,21 @@
       <c r="W77" s="23"/>
       <c r="X77" s="23"/>
       <c r="Y77" s="76"/>
-      <c r="Z77" s="132"/>
-      <c r="AA77" s="133"/>
-      <c r="AB77" s="124"/>
+      <c r="Z77" s="134"/>
+      <c r="AA77" s="135"/>
+      <c r="AB77" s="126"/>
       <c r="AC77" s="65"/>
       <c r="AD77" s="65"/>
     </row>
-    <row r="78" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="G78" s="9"/>
     </row>
-    <row r="79" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="80" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="81" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="82" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="83" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="84" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="50">
     <mergeCell ref="AB9:AB77"/>

</xml_diff>

<commit_message>
forcewave 20230503 쿼리 수정 중
</commit_message>
<xml_diff>
--- a/document/일정표_최경수.xlsx
+++ b/document/일정표_최경수.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\facci\Desktop\Dukkeobi\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797DC66F-082E-4084-9E88-EFF0349C97DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC36527-1F51-4CDA-993C-1025B01CEF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4F68EF3D-DEC7-4864-A746-04C7E98A59CC}"/>
   </bookViews>
@@ -1082,7 +1082,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1338,10 +1338,100 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1398,101 +1488,23 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1816,29 +1828,29 @@
   <dimension ref="A1:BT84"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V47" sqref="V47"/>
+      <pane ySplit="8" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA73" sqref="AA73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="19.899999999999999" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="19.899999999999999" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.08203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.08203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.08203125" style="4" customWidth="1"/>
-    <col min="7" max="8" width="3.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.125" style="4" customWidth="1"/>
+    <col min="7" max="8" width="3.125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="1.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="28" width="1.83203125" style="4" customWidth="1"/>
-    <col min="29" max="30" width="1.83203125" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="28" width="1.875" style="4" customWidth="1"/>
+    <col min="29" max="30" width="1.875" style="4" hidden="1" customWidth="1"/>
     <col min="31" max="70" width="8.75" style="1" hidden="1" customWidth="1"/>
     <col min="71" max="72" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="73" max="16384" width="8.75" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1853,30 +1865,30 @@
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="1"/>
-      <c r="J2" s="102" t="s">
+      <c r="J2" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="N2" s="88" t="s">
+      <c r="K2" s="132"/>
+      <c r="L2" s="132"/>
+      <c r="N2" s="118" t="s">
         <v>145</v>
       </c>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="89"/>
-      <c r="U2" s="89"/>
-      <c r="V2" s="89"/>
-      <c r="W2" s="89"/>
-      <c r="X2" s="89"/>
-      <c r="Y2" s="89"/>
-      <c r="Z2" s="89"/>
-      <c r="AA2" s="89"/>
-      <c r="AB2" s="90"/>
-    </row>
-    <row r="3" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="O2" s="119"/>
+      <c r="P2" s="119"/>
+      <c r="Q2" s="119"/>
+      <c r="R2" s="119"/>
+      <c r="S2" s="119"/>
+      <c r="T2" s="119"/>
+      <c r="U2" s="119"/>
+      <c r="V2" s="119"/>
+      <c r="W2" s="119"/>
+      <c r="X2" s="119"/>
+      <c r="Y2" s="119"/>
+      <c r="Z2" s="119"/>
+      <c r="AA2" s="119"/>
+      <c r="AB2" s="120"/>
+    </row>
+    <row r="3" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1891,28 +1903,28 @@
       </c>
       <c r="F3" s="71"/>
       <c r="G3" s="73"/>
-      <c r="J3" s="103" t="s">
+      <c r="J3" s="133" t="s">
         <v>121</v>
       </c>
-      <c r="K3" s="103"/>
-      <c r="L3" s="103"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="92"/>
-      <c r="S3" s="92"/>
-      <c r="T3" s="92"/>
-      <c r="U3" s="92"/>
-      <c r="V3" s="92"/>
-      <c r="W3" s="92"/>
-      <c r="X3" s="92"/>
-      <c r="Y3" s="92"/>
-      <c r="Z3" s="92"/>
-      <c r="AA3" s="92"/>
-      <c r="AB3" s="93"/>
-    </row>
-    <row r="4" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="K3" s="133"/>
+      <c r="L3" s="133"/>
+      <c r="N3" s="121"/>
+      <c r="O3" s="122"/>
+      <c r="P3" s="122"/>
+      <c r="Q3" s="122"/>
+      <c r="R3" s="122"/>
+      <c r="S3" s="122"/>
+      <c r="T3" s="122"/>
+      <c r="U3" s="122"/>
+      <c r="V3" s="122"/>
+      <c r="W3" s="122"/>
+      <c r="X3" s="122"/>
+      <c r="Y3" s="122"/>
+      <c r="Z3" s="122"/>
+      <c r="AA3" s="122"/>
+      <c r="AB3" s="123"/>
+    </row>
+    <row r="4" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1927,132 +1939,132 @@
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="1"/>
-      <c r="J4" s="104" t="s">
+      <c r="J4" s="134" t="s">
         <v>132</v>
       </c>
-      <c r="K4" s="104"/>
-      <c r="L4" s="104"/>
-      <c r="N4" s="94"/>
-      <c r="O4" s="95"/>
-      <c r="P4" s="95"/>
-      <c r="Q4" s="95"/>
-      <c r="R4" s="95"/>
-      <c r="S4" s="95"/>
-      <c r="T4" s="95"/>
-      <c r="U4" s="95"/>
-      <c r="V4" s="95"/>
-      <c r="W4" s="95"/>
-      <c r="X4" s="95"/>
-      <c r="Y4" s="95"/>
-      <c r="Z4" s="95"/>
-      <c r="AA4" s="95"/>
-      <c r="AB4" s="96"/>
-    </row>
-    <row r="5" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="K4" s="134"/>
+      <c r="L4" s="134"/>
+      <c r="N4" s="124"/>
+      <c r="O4" s="125"/>
+      <c r="P4" s="125"/>
+      <c r="Q4" s="125"/>
+      <c r="R4" s="125"/>
+      <c r="S4" s="125"/>
+      <c r="T4" s="125"/>
+      <c r="U4" s="125"/>
+      <c r="V4" s="125"/>
+      <c r="W4" s="125"/>
+      <c r="X4" s="125"/>
+      <c r="Y4" s="125"/>
+      <c r="Z4" s="125"/>
+      <c r="AA4" s="125"/>
+      <c r="AB4" s="126"/>
+    </row>
+    <row r="5" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:30" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="116" t="s">
+    <row r="6" spans="1:30" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="112" t="s">
         <v>152</v>
       </c>
-      <c r="C6" s="105" t="s">
+      <c r="C6" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="105" t="s">
+      <c r="D6" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="105" t="s">
+      <c r="E6" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="105" t="s">
+      <c r="F6" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="105" t="s">
+      <c r="G6" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="97" t="s">
+      <c r="H6" s="127" t="s">
         <v>151</v>
       </c>
       <c r="I6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="99" t="s">
+      <c r="J6" s="129" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="99"/>
-      <c r="L6" s="99"/>
-      <c r="M6" s="99"/>
-      <c r="N6" s="99"/>
-      <c r="O6" s="99"/>
-      <c r="P6" s="99"/>
-      <c r="Q6" s="99"/>
-      <c r="R6" s="99"/>
-      <c r="S6" s="99"/>
-      <c r="T6" s="99"/>
-      <c r="U6" s="99"/>
-      <c r="V6" s="99"/>
-      <c r="W6" s="100"/>
-      <c r="X6" s="101" t="s">
+      <c r="K6" s="129"/>
+      <c r="L6" s="129"/>
+      <c r="M6" s="129"/>
+      <c r="N6" s="129"/>
+      <c r="O6" s="129"/>
+      <c r="P6" s="129"/>
+      <c r="Q6" s="129"/>
+      <c r="R6" s="129"/>
+      <c r="S6" s="129"/>
+      <c r="T6" s="129"/>
+      <c r="U6" s="129"/>
+      <c r="V6" s="129"/>
+      <c r="W6" s="130"/>
+      <c r="X6" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="Y6" s="99"/>
-      <c r="Z6" s="99"/>
-      <c r="AA6" s="99"/>
-      <c r="AB6" s="99"/>
-      <c r="AC6" s="99"/>
-      <c r="AD6" s="100"/>
-    </row>
-    <row r="7" spans="1:30" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="Y6" s="129"/>
+      <c r="Z6" s="129"/>
+      <c r="AA6" s="129"/>
+      <c r="AB6" s="129"/>
+      <c r="AC6" s="129"/>
+      <c r="AD6" s="130"/>
+    </row>
+    <row r="7" spans="1:30" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="117"/>
-      <c r="C7" s="105"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="105"/>
-      <c r="F7" s="105"/>
-      <c r="G7" s="105"/>
-      <c r="H7" s="98"/>
+      <c r="B7" s="113"/>
+      <c r="C7" s="111"/>
+      <c r="D7" s="111"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="128"/>
       <c r="I7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="86" t="s">
+      <c r="J7" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="86"/>
-      <c r="L7" s="86"/>
-      <c r="M7" s="86"/>
-      <c r="N7" s="86"/>
-      <c r="O7" s="86"/>
-      <c r="P7" s="86"/>
-      <c r="Q7" s="85" t="s">
+      <c r="K7" s="115"/>
+      <c r="L7" s="115"/>
+      <c r="M7" s="115"/>
+      <c r="N7" s="115"/>
+      <c r="O7" s="115"/>
+      <c r="P7" s="115"/>
+      <c r="Q7" s="116" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="86"/>
-      <c r="S7" s="86"/>
-      <c r="T7" s="86"/>
-      <c r="U7" s="86"/>
-      <c r="V7" s="86"/>
-      <c r="W7" s="86"/>
-      <c r="X7" s="85" t="s">
+      <c r="R7" s="115"/>
+      <c r="S7" s="115"/>
+      <c r="T7" s="115"/>
+      <c r="U7" s="115"/>
+      <c r="V7" s="115"/>
+      <c r="W7" s="115"/>
+      <c r="X7" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="Y7" s="86"/>
-      <c r="Z7" s="86"/>
-      <c r="AA7" s="86"/>
-      <c r="AB7" s="86"/>
-      <c r="AC7" s="86"/>
-      <c r="AD7" s="87"/>
-    </row>
-    <row r="8" spans="1:30" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="Y7" s="115"/>
+      <c r="Z7" s="115"/>
+      <c r="AA7" s="115"/>
+      <c r="AB7" s="115"/>
+      <c r="AC7" s="115"/>
+      <c r="AD7" s="117"/>
+    </row>
+    <row r="8" spans="1:30" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="118"/>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="105"/>
-      <c r="G8" s="105"/>
-      <c r="H8" s="98"/>
+      <c r="B8" s="114"/>
+      <c r="C8" s="111"/>
+      <c r="D8" s="111"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="128"/>
       <c r="I8" s="13" t="s">
         <v>13</v>
       </c>
@@ -2120,11 +2132,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="119" t="s">
+    <row r="9" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="101" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="98" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="14" t="s">
@@ -2161,15 +2173,15 @@
       <c r="Y9" s="14"/>
       <c r="Z9" s="14"/>
       <c r="AA9" s="14"/>
-      <c r="AB9" s="124" t="s">
+      <c r="AB9" s="86" t="s">
         <v>133</v>
       </c>
       <c r="AC9" s="53"/>
       <c r="AD9" s="54"/>
     </row>
-    <row r="10" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="109"/>
-      <c r="C10" s="114"/>
+    <row r="10" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="102"/>
+      <c r="C10" s="99"/>
       <c r="D10" s="18" t="s">
         <v>81</v>
       </c>
@@ -2204,13 +2216,13 @@
       <c r="Y10" s="18"/>
       <c r="Z10" s="18"/>
       <c r="AA10" s="18"/>
-      <c r="AB10" s="125"/>
+      <c r="AB10" s="87"/>
       <c r="AC10" s="55"/>
       <c r="AD10" s="56"/>
     </row>
-    <row r="11" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="109"/>
-      <c r="C11" s="115"/>
+    <row r="11" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="102"/>
+      <c r="C11" s="100"/>
       <c r="D11" s="22" t="s">
         <v>82</v>
       </c>
@@ -2245,16 +2257,16 @@
       <c r="Y11" s="22"/>
       <c r="Z11" s="22"/>
       <c r="AA11" s="22"/>
-      <c r="AB11" s="125"/>
+      <c r="AB11" s="87"/>
       <c r="AC11" s="57"/>
       <c r="AD11" s="58"/>
     </row>
-    <row r="12" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="109"/>
-      <c r="C12" s="113" t="s">
+    <row r="12" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="102"/>
+      <c r="C12" s="98" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="123" t="s">
+      <c r="D12" s="107" t="s">
         <v>83</v>
       </c>
       <c r="E12" s="14" t="s">
@@ -2286,14 +2298,14 @@
       <c r="Y12" s="14"/>
       <c r="Z12" s="14"/>
       <c r="AA12" s="14"/>
-      <c r="AB12" s="125"/>
+      <c r="AB12" s="87"/>
       <c r="AC12" s="53"/>
       <c r="AD12" s="54"/>
     </row>
-    <row r="13" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="109"/>
-      <c r="C13" s="114"/>
-      <c r="D13" s="111"/>
+    <row r="13" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="102"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="96"/>
       <c r="E13" s="18" t="s">
         <v>64</v>
       </c>
@@ -2323,14 +2335,14 @@
       <c r="Y13" s="18"/>
       <c r="Z13" s="18"/>
       <c r="AA13" s="18"/>
-      <c r="AB13" s="125"/>
+      <c r="AB13" s="87"/>
       <c r="AC13" s="55"/>
       <c r="AD13" s="56"/>
     </row>
-    <row r="14" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="109"/>
-      <c r="C14" s="114"/>
-      <c r="D14" s="111"/>
+    <row r="14" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="102"/>
+      <c r="C14" s="99"/>
+      <c r="D14" s="96"/>
       <c r="E14" s="18" t="s">
         <v>65</v>
       </c>
@@ -2360,14 +2372,14 @@
       <c r="Y14" s="18"/>
       <c r="Z14" s="18"/>
       <c r="AA14" s="18"/>
-      <c r="AB14" s="125"/>
+      <c r="AB14" s="87"/>
       <c r="AC14" s="55"/>
       <c r="AD14" s="56"/>
     </row>
-    <row r="15" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="109"/>
-      <c r="C15" s="114"/>
-      <c r="D15" s="111"/>
+    <row r="15" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="102"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="96"/>
       <c r="E15" s="18" t="s">
         <v>72</v>
       </c>
@@ -2397,14 +2409,14 @@
       <c r="Y15" s="18"/>
       <c r="Z15" s="18"/>
       <c r="AA15" s="18"/>
-      <c r="AB15" s="125"/>
+      <c r="AB15" s="87"/>
       <c r="AC15" s="55"/>
       <c r="AD15" s="56"/>
     </row>
-    <row r="16" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="109"/>
-      <c r="C16" s="114"/>
-      <c r="D16" s="111"/>
+    <row r="16" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="102"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="96"/>
       <c r="E16" s="18" t="s">
         <v>66</v>
       </c>
@@ -2434,14 +2446,14 @@
       <c r="Y16" s="18"/>
       <c r="Z16" s="18"/>
       <c r="AA16" s="18"/>
-      <c r="AB16" s="125"/>
+      <c r="AB16" s="87"/>
       <c r="AC16" s="55"/>
       <c r="AD16" s="56"/>
     </row>
-    <row r="17" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="109"/>
-      <c r="C17" s="114"/>
-      <c r="D17" s="111"/>
+    <row r="17" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="102"/>
+      <c r="C17" s="99"/>
+      <c r="D17" s="96"/>
       <c r="E17" s="18" t="s">
         <v>67</v>
       </c>
@@ -2471,14 +2483,14 @@
       <c r="Y17" s="18"/>
       <c r="Z17" s="18"/>
       <c r="AA17" s="18"/>
-      <c r="AB17" s="125"/>
+      <c r="AB17" s="87"/>
       <c r="AC17" s="55"/>
       <c r="AD17" s="56"/>
     </row>
-    <row r="18" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="109"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="111"/>
+    <row r="18" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="102"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="96"/>
       <c r="E18" s="18" t="s">
         <v>68</v>
       </c>
@@ -2508,14 +2520,14 @@
       <c r="Y18" s="18"/>
       <c r="Z18" s="18"/>
       <c r="AA18" s="18"/>
-      <c r="AB18" s="125"/>
+      <c r="AB18" s="87"/>
       <c r="AC18" s="55"/>
       <c r="AD18" s="56"/>
     </row>
-    <row r="19" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="109"/>
-      <c r="C19" s="114"/>
-      <c r="D19" s="111"/>
+    <row r="19" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="102"/>
+      <c r="C19" s="99"/>
+      <c r="D19" s="96"/>
       <c r="E19" s="18" t="s">
         <v>69</v>
       </c>
@@ -2545,14 +2557,14 @@
       <c r="Y19" s="18"/>
       <c r="Z19" s="18"/>
       <c r="AA19" s="18"/>
-      <c r="AB19" s="125"/>
+      <c r="AB19" s="87"/>
       <c r="AC19" s="55"/>
       <c r="AD19" s="56"/>
     </row>
-    <row r="20" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="109"/>
-      <c r="C20" s="115"/>
-      <c r="D20" s="112"/>
+    <row r="20" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="102"/>
+      <c r="C20" s="100"/>
+      <c r="D20" s="97"/>
       <c r="E20" s="22" t="s">
         <v>70</v>
       </c>
@@ -2582,12 +2594,12 @@
       <c r="Y20" s="22"/>
       <c r="Z20" s="22"/>
       <c r="AA20" s="22"/>
-      <c r="AB20" s="125"/>
+      <c r="AB20" s="87"/>
       <c r="AC20" s="57"/>
       <c r="AD20" s="58"/>
     </row>
-    <row r="21" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B21" s="109"/>
+    <row r="21" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="102"/>
       <c r="C21" s="36" t="s">
         <v>59</v>
       </c>
@@ -2625,12 +2637,12 @@
       <c r="Y21" s="18"/>
       <c r="Z21" s="18"/>
       <c r="AA21" s="18"/>
-      <c r="AB21" s="125"/>
+      <c r="AB21" s="87"/>
       <c r="AC21" s="55"/>
       <c r="AD21" s="56"/>
     </row>
-    <row r="22" spans="2:30" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B22" s="110"/>
+    <row r="22" spans="2:30" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="103"/>
       <c r="C22" s="68" t="s">
         <v>135</v>
       </c>
@@ -2667,19 +2679,19 @@
       <c r="X22" s="26"/>
       <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
-      <c r="AA22" s="42"/>
-      <c r="AB22" s="125"/>
+      <c r="AA22" s="78"/>
+      <c r="AB22" s="87"/>
       <c r="AC22" s="59"/>
       <c r="AD22" s="60"/>
     </row>
-    <row r="23" spans="2:30" ht="19.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="109" t="s">
+    <row r="23" spans="2:30" ht="19.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="102" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="120" t="s">
+      <c r="C23" s="104" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="122" t="s">
+      <c r="D23" s="106" t="s">
         <v>73</v>
       </c>
       <c r="E23" s="30" t="s">
@@ -2713,14 +2725,14 @@
       <c r="Y23" s="30"/>
       <c r="Z23" s="30"/>
       <c r="AA23" s="30"/>
-      <c r="AB23" s="125"/>
+      <c r="AB23" s="87"/>
       <c r="AC23" s="61"/>
       <c r="AD23" s="62"/>
     </row>
-    <row r="24" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="109"/>
-      <c r="C24" s="121"/>
-      <c r="D24" s="111"/>
+    <row r="24" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="102"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="96"/>
       <c r="E24" s="18" t="s">
         <v>75</v>
       </c>
@@ -2752,14 +2764,14 @@
       <c r="Y24" s="18"/>
       <c r="Z24" s="18"/>
       <c r="AA24" s="18"/>
-      <c r="AB24" s="125"/>
+      <c r="AB24" s="87"/>
       <c r="AC24" s="55"/>
       <c r="AD24" s="56"/>
     </row>
-    <row r="25" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="109"/>
-      <c r="C25" s="121"/>
-      <c r="D25" s="111"/>
+    <row r="25" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="102"/>
+      <c r="C25" s="105"/>
+      <c r="D25" s="96"/>
       <c r="E25" s="18" t="s">
         <v>141</v>
       </c>
@@ -2791,12 +2803,12 @@
       <c r="Y25" s="18"/>
       <c r="Z25" s="18"/>
       <c r="AA25" s="18"/>
-      <c r="AB25" s="125"/>
+      <c r="AB25" s="87"/>
       <c r="AC25" s="55"/>
       <c r="AD25" s="56"/>
     </row>
-    <row r="26" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="109"/>
+    <row r="26" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="102"/>
       <c r="C26" s="38" t="s">
         <v>54</v>
       </c>
@@ -2834,12 +2846,12 @@
       <c r="Y26" s="18"/>
       <c r="Z26" s="18"/>
       <c r="AA26" s="18"/>
-      <c r="AB26" s="125"/>
+      <c r="AB26" s="87"/>
       <c r="AC26" s="55"/>
       <c r="AD26" s="56"/>
     </row>
-    <row r="27" spans="2:30" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B27" s="110"/>
+    <row r="27" spans="2:30" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="103"/>
       <c r="C27" s="37" t="s">
         <v>55</v>
       </c>
@@ -2877,12 +2889,12 @@
       <c r="Y27" s="26"/>
       <c r="Z27" s="26"/>
       <c r="AA27" s="26"/>
-      <c r="AB27" s="125"/>
+      <c r="AB27" s="87"/>
       <c r="AC27" s="59"/>
       <c r="AD27" s="60"/>
     </row>
-    <row r="28" spans="2:30" ht="19.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="108" t="s">
+    <row r="28" spans="2:30" ht="19.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="110" t="s">
         <v>123</v>
       </c>
       <c r="C28" s="38" t="s">
@@ -2914,19 +2926,19 @@
       <c r="R28" s="78"/>
       <c r="S28" s="18"/>
       <c r="T28" s="18"/>
-      <c r="U28" s="18"/>
-      <c r="V28" s="18"/>
-      <c r="W28" s="18"/>
+      <c r="U28" s="78"/>
+      <c r="V28" s="78"/>
+      <c r="W28" s="78"/>
       <c r="X28" s="18"/>
       <c r="Y28" s="18"/>
       <c r="Z28" s="18"/>
       <c r="AA28" s="18"/>
-      <c r="AB28" s="125"/>
+      <c r="AB28" s="87"/>
       <c r="AC28" s="55"/>
       <c r="AD28" s="55"/>
     </row>
-    <row r="29" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="109"/>
+    <row r="29" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="102"/>
       <c r="C29" s="38" t="s">
         <v>125</v>
       </c>
@@ -2963,12 +2975,12 @@
       <c r="Y29" s="18"/>
       <c r="Z29" s="18"/>
       <c r="AA29" s="18"/>
-      <c r="AB29" s="125"/>
+      <c r="AB29" s="87"/>
       <c r="AC29" s="55"/>
       <c r="AD29" s="55"/>
     </row>
-    <row r="30" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="109"/>
+    <row r="30" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="102"/>
       <c r="C30" s="38" t="s">
         <v>126</v>
       </c>
@@ -2996,21 +3008,20 @@
       <c r="P30" s="18"/>
       <c r="Q30" s="18"/>
       <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
       <c r="T30" s="18"/>
-      <c r="U30" s="18"/>
-      <c r="V30" s="18"/>
+      <c r="U30" s="78"/>
+      <c r="V30" s="78"/>
       <c r="W30" s="18"/>
       <c r="X30" s="18"/>
       <c r="Y30" s="18"/>
       <c r="Z30" s="18"/>
       <c r="AA30" s="18"/>
-      <c r="AB30" s="125"/>
+      <c r="AB30" s="87"/>
       <c r="AC30" s="55"/>
       <c r="AD30" s="55"/>
     </row>
-    <row r="31" spans="2:30" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B31" s="110"/>
+    <row r="31" spans="2:30" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="103"/>
       <c r="C31" s="37" t="s">
         <v>83</v>
       </c>
@@ -3043,26 +3054,26 @@
       <c r="T31" s="26"/>
       <c r="U31" s="26"/>
       <c r="V31" s="26"/>
-      <c r="W31" s="26"/>
+      <c r="W31" s="78"/>
       <c r="X31" s="26"/>
       <c r="Y31" s="26"/>
       <c r="Z31" s="26"/>
       <c r="AA31" s="26"/>
-      <c r="AB31" s="125"/>
+      <c r="AB31" s="87"/>
       <c r="AC31" s="59"/>
       <c r="AD31" s="59"/>
     </row>
-    <row r="32" spans="2:30" ht="19.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="106" t="s">
+    <row r="32" spans="2:30" ht="19.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="114" t="s">
+      <c r="C32" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="127" t="s">
+      <c r="D32" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="127"/>
+      <c r="E32" s="89"/>
       <c r="F32" s="19" t="s">
         <v>14</v>
       </c>
@@ -3087,17 +3098,17 @@
       <c r="W32" s="19"/>
       <c r="X32" s="19"/>
       <c r="Y32" s="19"/>
-      <c r="Z32" s="130" t="s">
+      <c r="Z32" s="92" t="s">
         <v>134</v>
       </c>
-      <c r="AA32" s="131"/>
-      <c r="AB32" s="125"/>
+      <c r="AA32" s="93"/>
+      <c r="AB32" s="87"/>
       <c r="AC32" s="63"/>
       <c r="AD32" s="64"/>
     </row>
-    <row r="33" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="106"/>
-      <c r="C33" s="114"/>
+    <row r="33" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="108"/>
+      <c r="C33" s="99"/>
       <c r="D33" s="18" t="s">
         <v>24</v>
       </c>
@@ -3128,15 +3139,15 @@
       <c r="W33" s="19"/>
       <c r="X33" s="19"/>
       <c r="Y33" s="19"/>
-      <c r="Z33" s="132"/>
-      <c r="AA33" s="133"/>
-      <c r="AB33" s="125"/>
+      <c r="Z33" s="94"/>
+      <c r="AA33" s="95"/>
+      <c r="AB33" s="87"/>
       <c r="AC33" s="63"/>
       <c r="AD33" s="64"/>
     </row>
-    <row r="34" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="106"/>
-      <c r="C34" s="114"/>
+    <row r="34" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="108"/>
+      <c r="C34" s="99"/>
       <c r="D34" s="18" t="s">
         <v>23</v>
       </c>
@@ -3167,15 +3178,15 @@
       <c r="W34" s="19"/>
       <c r="X34" s="19"/>
       <c r="Y34" s="19"/>
-      <c r="Z34" s="132"/>
-      <c r="AA34" s="133"/>
-      <c r="AB34" s="125"/>
+      <c r="Z34" s="94"/>
+      <c r="AA34" s="95"/>
+      <c r="AB34" s="87"/>
       <c r="AC34" s="63"/>
       <c r="AD34" s="64"/>
     </row>
-    <row r="35" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="106"/>
-      <c r="C35" s="114"/>
+    <row r="35" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="108"/>
+      <c r="C35" s="99"/>
       <c r="D35" s="18" t="s">
         <v>26</v>
       </c>
@@ -3206,16 +3217,16 @@
       <c r="W35" s="19"/>
       <c r="X35" s="19"/>
       <c r="Y35" s="19"/>
-      <c r="Z35" s="132"/>
-      <c r="AA35" s="133"/>
-      <c r="AB35" s="125"/>
+      <c r="Z35" s="94"/>
+      <c r="AA35" s="95"/>
+      <c r="AB35" s="87"/>
       <c r="AC35" s="63"/>
       <c r="AD35" s="64"/>
     </row>
-    <row r="36" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="106"/>
-      <c r="C36" s="114"/>
-      <c r="D36" s="111" t="s">
+    <row r="36" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="108"/>
+      <c r="C36" s="99"/>
+      <c r="D36" s="96" t="s">
         <v>28</v>
       </c>
       <c r="E36" s="18" t="s">
@@ -3245,16 +3256,16 @@
       <c r="W36" s="19"/>
       <c r="X36" s="19"/>
       <c r="Y36" s="19"/>
-      <c r="Z36" s="132"/>
-      <c r="AA36" s="133"/>
-      <c r="AB36" s="125"/>
+      <c r="Z36" s="135"/>
+      <c r="AA36" s="136"/>
+      <c r="AB36" s="87"/>
       <c r="AC36" s="63"/>
       <c r="AD36" s="64"/>
     </row>
-    <row r="37" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="106"/>
-      <c r="C37" s="114"/>
-      <c r="D37" s="111"/>
+    <row r="37" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="108"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="96"/>
       <c r="E37" s="18" t="s">
         <v>30</v>
       </c>
@@ -3282,16 +3293,16 @@
       <c r="W37" s="19"/>
       <c r="X37" s="19"/>
       <c r="Y37" s="19"/>
-      <c r="Z37" s="132"/>
-      <c r="AA37" s="133"/>
-      <c r="AB37" s="125"/>
+      <c r="Z37" s="135"/>
+      <c r="AA37" s="136"/>
+      <c r="AB37" s="87"/>
       <c r="AC37" s="63"/>
       <c r="AD37" s="64"/>
     </row>
-    <row r="38" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="106"/>
-      <c r="C38" s="115"/>
-      <c r="D38" s="112"/>
+    <row r="38" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="108"/>
+      <c r="C38" s="100"/>
+      <c r="D38" s="97"/>
       <c r="E38" s="22" t="s">
         <v>31</v>
       </c>
@@ -3319,21 +3330,21 @@
       <c r="W38" s="23"/>
       <c r="X38" s="23"/>
       <c r="Y38" s="23"/>
-      <c r="Z38" s="132"/>
-      <c r="AA38" s="133"/>
-      <c r="AB38" s="125"/>
+      <c r="Z38" s="135"/>
+      <c r="AA38" s="136"/>
+      <c r="AB38" s="87"/>
       <c r="AC38" s="65"/>
       <c r="AD38" s="66"/>
     </row>
-    <row r="39" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="106"/>
-      <c r="C39" s="113" t="s">
+    <row r="39" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="108"/>
+      <c r="C39" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="128" t="s">
+      <c r="D39" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="E39" s="128"/>
+      <c r="E39" s="90"/>
       <c r="F39" s="15" t="s">
         <v>14</v>
       </c>
@@ -3353,22 +3364,22 @@
       <c r="P39" s="49"/>
       <c r="Q39" s="11"/>
       <c r="R39" s="15"/>
-      <c r="S39" s="136"/>
+      <c r="S39" s="85"/>
       <c r="T39" s="15"/>
       <c r="U39" s="51"/>
       <c r="V39" s="15"/>
       <c r="W39" s="15"/>
       <c r="X39" s="15"/>
       <c r="Y39" s="31"/>
-      <c r="Z39" s="132"/>
-      <c r="AA39" s="133"/>
-      <c r="AB39" s="125"/>
+      <c r="Z39" s="135"/>
+      <c r="AA39" s="136"/>
+      <c r="AB39" s="87"/>
       <c r="AC39" s="63"/>
       <c r="AD39" s="63"/>
     </row>
-    <row r="40" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="106"/>
-      <c r="C40" s="114"/>
+    <row r="40" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="108"/>
+      <c r="C40" s="99"/>
       <c r="D40" s="18" t="s">
         <v>35</v>
       </c>
@@ -3400,15 +3411,15 @@
       <c r="W40" s="19"/>
       <c r="X40" s="19"/>
       <c r="Y40" s="32"/>
-      <c r="Z40" s="132"/>
-      <c r="AA40" s="133"/>
-      <c r="AB40" s="125"/>
+      <c r="Z40" s="135"/>
+      <c r="AA40" s="136"/>
+      <c r="AB40" s="87"/>
       <c r="AC40" s="63"/>
       <c r="AD40" s="63"/>
     </row>
-    <row r="41" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="106"/>
-      <c r="C41" s="114"/>
+    <row r="41" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="108"/>
+      <c r="C41" s="99"/>
       <c r="D41" s="18" t="s">
         <v>36</v>
       </c>
@@ -3440,15 +3451,15 @@
       <c r="W41" s="19"/>
       <c r="X41" s="19"/>
       <c r="Y41" s="32"/>
-      <c r="Z41" s="132"/>
-      <c r="AA41" s="133"/>
-      <c r="AB41" s="125"/>
+      <c r="Z41" s="135"/>
+      <c r="AA41" s="136"/>
+      <c r="AB41" s="87"/>
       <c r="AC41" s="63"/>
       <c r="AD41" s="63"/>
     </row>
-    <row r="42" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="106"/>
-      <c r="C42" s="114"/>
+    <row r="42" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="108"/>
+      <c r="C42" s="99"/>
       <c r="D42" s="18" t="s">
         <v>39</v>
       </c>
@@ -3475,21 +3486,21 @@
       <c r="R42" s="19"/>
       <c r="S42" s="84"/>
       <c r="T42" s="19"/>
-      <c r="U42" s="50"/>
-      <c r="V42" s="19"/>
+      <c r="U42" s="52"/>
+      <c r="V42" s="23"/>
       <c r="W42" s="19"/>
       <c r="X42" s="19"/>
       <c r="Y42" s="32"/>
-      <c r="Z42" s="132"/>
-      <c r="AA42" s="133"/>
-      <c r="AB42" s="125"/>
+      <c r="Z42" s="135"/>
+      <c r="AA42" s="136"/>
+      <c r="AB42" s="87"/>
       <c r="AC42" s="63"/>
       <c r="AD42" s="63"/>
     </row>
-    <row r="43" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="106"/>
-      <c r="C43" s="114"/>
-      <c r="D43" s="111" t="s">
+    <row r="43" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="108"/>
+      <c r="C43" s="99"/>
+      <c r="D43" s="96" t="s">
         <v>41</v>
       </c>
       <c r="E43" s="18" t="s">
@@ -3518,16 +3529,16 @@
       <c r="W43" s="19"/>
       <c r="X43" s="19"/>
       <c r="Y43" s="32"/>
-      <c r="Z43" s="132"/>
-      <c r="AA43" s="133"/>
-      <c r="AB43" s="125"/>
+      <c r="Z43" s="135"/>
+      <c r="AA43" s="136"/>
+      <c r="AB43" s="87"/>
       <c r="AC43" s="63"/>
       <c r="AD43" s="63"/>
     </row>
-    <row r="44" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="106"/>
-      <c r="C44" s="115"/>
-      <c r="D44" s="112"/>
+    <row r="44" spans="2:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="108"/>
+      <c r="C44" s="100"/>
+      <c r="D44" s="97"/>
       <c r="E44" s="22" t="s">
         <v>43</v>
       </c>
@@ -3555,21 +3566,21 @@
       <c r="W44" s="23"/>
       <c r="X44" s="23"/>
       <c r="Y44" s="33"/>
-      <c r="Z44" s="132"/>
-      <c r="AA44" s="133"/>
-      <c r="AB44" s="125"/>
+      <c r="Z44" s="135"/>
+      <c r="AA44" s="136"/>
+      <c r="AB44" s="87"/>
       <c r="AC44" s="65"/>
       <c r="AD44" s="65"/>
     </row>
-    <row r="45" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="106"/>
-      <c r="C45" s="113" t="s">
+    <row r="45" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="108"/>
+      <c r="C45" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="D45" s="129" t="s">
+      <c r="D45" s="91" t="s">
         <v>146</v>
       </c>
-      <c r="E45" s="129"/>
+      <c r="E45" s="91"/>
       <c r="F45" s="15" t="s">
         <v>14</v>
       </c>
@@ -3589,23 +3600,23 @@
       <c r="P45" s="49"/>
       <c r="Q45" s="11"/>
       <c r="R45" s="15"/>
-      <c r="S45" s="136"/>
-      <c r="T45" s="136"/>
-      <c r="U45" s="15"/>
-      <c r="V45" s="51"/>
+      <c r="S45" s="85"/>
+      <c r="T45" s="85"/>
+      <c r="U45" s="78"/>
+      <c r="V45" s="78"/>
       <c r="W45" s="15"/>
       <c r="X45" s="15"/>
       <c r="Y45" s="31"/>
-      <c r="Z45" s="132"/>
-      <c r="AA45" s="133"/>
-      <c r="AB45" s="125"/>
+      <c r="Z45" s="135"/>
+      <c r="AA45" s="136"/>
+      <c r="AB45" s="87"/>
       <c r="AC45" s="63"/>
       <c r="AD45" s="63"/>
     </row>
-    <row r="46" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="106"/>
-      <c r="C46" s="114"/>
-      <c r="D46" s="111" t="s">
+    <row r="46" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="108"/>
+      <c r="C46" s="99"/>
+      <c r="D46" s="96" t="s">
         <v>45</v>
       </c>
       <c r="E46" s="18" t="s">
@@ -3635,16 +3646,16 @@
       <c r="W46" s="19"/>
       <c r="X46" s="19"/>
       <c r="Y46" s="32"/>
-      <c r="Z46" s="132"/>
-      <c r="AA46" s="133"/>
-      <c r="AB46" s="125"/>
+      <c r="Z46" s="135"/>
+      <c r="AA46" s="136"/>
+      <c r="AB46" s="87"/>
       <c r="AC46" s="63"/>
       <c r="AD46" s="63"/>
     </row>
-    <row r="47" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B47" s="106"/>
-      <c r="C47" s="114"/>
-      <c r="D47" s="111"/>
+    <row r="47" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="108"/>
+      <c r="C47" s="99"/>
+      <c r="D47" s="96"/>
       <c r="E47" s="18" t="s">
         <v>47</v>
       </c>
@@ -3672,16 +3683,16 @@
       <c r="W47" s="19"/>
       <c r="X47" s="19"/>
       <c r="Y47" s="32"/>
-      <c r="Z47" s="132"/>
-      <c r="AA47" s="133"/>
-      <c r="AB47" s="125"/>
+      <c r="Z47" s="135"/>
+      <c r="AA47" s="136"/>
+      <c r="AB47" s="87"/>
       <c r="AC47" s="63"/>
       <c r="AD47" s="63"/>
     </row>
-    <row r="48" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="106"/>
-      <c r="C48" s="114"/>
-      <c r="D48" s="111"/>
+    <row r="48" spans="2:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="108"/>
+      <c r="C48" s="99"/>
+      <c r="D48" s="96"/>
       <c r="E48" s="18" t="s">
         <v>48</v>
       </c>
@@ -3704,21 +3715,21 @@
       <c r="P48" s="47"/>
       <c r="R48" s="19"/>
       <c r="T48" s="84"/>
-      <c r="U48" s="19"/>
-      <c r="V48" s="50"/>
+      <c r="U48" s="78"/>
+      <c r="V48" s="78"/>
       <c r="W48" s="19"/>
       <c r="X48" s="19"/>
       <c r="Y48" s="32"/>
-      <c r="Z48" s="132"/>
-      <c r="AA48" s="133"/>
-      <c r="AB48" s="125"/>
+      <c r="Z48" s="135"/>
+      <c r="AA48" s="136"/>
+      <c r="AB48" s="87"/>
       <c r="AC48" s="63"/>
       <c r="AD48" s="63"/>
     </row>
-    <row r="49" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="106"/>
-      <c r="C49" s="114"/>
-      <c r="D49" s="111"/>
+    <row r="49" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="108"/>
+      <c r="C49" s="99"/>
+      <c r="D49" s="96"/>
       <c r="E49" s="18" t="s">
         <v>131</v>
       </c>
@@ -3741,20 +3752,20 @@
       <c r="P49" s="47"/>
       <c r="R49" s="19"/>
       <c r="T49" s="84"/>
-      <c r="U49" s="19"/>
-      <c r="V49" s="50"/>
-      <c r="W49" s="19"/>
+      <c r="U49" s="78"/>
+      <c r="V49" s="79"/>
+      <c r="W49" s="23"/>
       <c r="X49" s="19"/>
       <c r="Y49" s="32"/>
-      <c r="Z49" s="132"/>
-      <c r="AA49" s="133"/>
-      <c r="AB49" s="125"/>
+      <c r="Z49" s="135"/>
+      <c r="AA49" s="136"/>
+      <c r="AB49" s="87"/>
       <c r="AC49" s="63"/>
       <c r="AD49" s="63"/>
     </row>
-    <row r="50" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="106"/>
-      <c r="C50" s="115"/>
+    <row r="50" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="108"/>
+      <c r="C50" s="100"/>
       <c r="D50" s="22" t="s">
         <v>49</v>
       </c>
@@ -3785,22 +3796,22 @@
       <c r="W50" s="23"/>
       <c r="X50" s="23"/>
       <c r="Y50" s="33"/>
-      <c r="Z50" s="132"/>
-      <c r="AA50" s="133"/>
-      <c r="AB50" s="125"/>
+      <c r="Z50" s="135"/>
+      <c r="AA50" s="136"/>
+      <c r="AB50" s="87"/>
       <c r="AC50" s="63"/>
       <c r="AD50" s="63"/>
     </row>
-    <row r="51" spans="1:30" s="10" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:30" s="10" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
-      <c r="B51" s="106"/>
-      <c r="C51" s="113" t="s">
+      <c r="B51" s="108"/>
+      <c r="C51" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="D51" s="129" t="s">
+      <c r="D51" s="91" t="s">
         <v>91</v>
       </c>
-      <c r="E51" s="129"/>
+      <c r="E51" s="91"/>
       <c r="F51" s="19" t="s">
         <v>14</v>
       </c>
@@ -3820,20 +3831,20 @@
       <c r="P51" s="15"/>
       <c r="Q51" s="49"/>
       <c r="R51" s="49"/>
-      <c r="V51" s="51"/>
-      <c r="W51" s="15"/>
+      <c r="V51" s="78"/>
+      <c r="W51" s="78"/>
       <c r="X51" s="15"/>
       <c r="Y51" s="15"/>
-      <c r="Z51" s="132"/>
-      <c r="AA51" s="133"/>
-      <c r="AB51" s="125"/>
+      <c r="Z51" s="135"/>
+      <c r="AA51" s="136"/>
+      <c r="AB51" s="87"/>
       <c r="AC51" s="67"/>
       <c r="AD51" s="67"/>
     </row>
-    <row r="52" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="106"/>
-      <c r="C52" s="114"/>
-      <c r="D52" s="111" t="s">
+    <row r="52" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="108"/>
+      <c r="C52" s="99"/>
+      <c r="D52" s="96" t="s">
         <v>85</v>
       </c>
       <c r="E52" s="18" t="s">
@@ -3858,20 +3869,20 @@
       <c r="P52" s="19"/>
       <c r="Q52" s="47"/>
       <c r="R52" s="19"/>
-      <c r="V52" s="50"/>
+      <c r="V52" s="78"/>
       <c r="W52" s="19"/>
       <c r="X52" s="19"/>
       <c r="Y52" s="19"/>
-      <c r="Z52" s="132"/>
-      <c r="AA52" s="133"/>
-      <c r="AB52" s="125"/>
+      <c r="Z52" s="135"/>
+      <c r="AA52" s="136"/>
+      <c r="AB52" s="87"/>
       <c r="AC52" s="63"/>
       <c r="AD52" s="63"/>
     </row>
-    <row r="53" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="106"/>
-      <c r="C53" s="114"/>
-      <c r="D53" s="111"/>
+    <row r="53" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="108"/>
+      <c r="C53" s="99"/>
+      <c r="D53" s="96"/>
       <c r="E53" s="18" t="s">
         <v>87</v>
       </c>
@@ -3894,20 +3905,20 @@
       <c r="P53" s="19"/>
       <c r="Q53" s="47"/>
       <c r="R53" s="19"/>
-      <c r="V53" s="50"/>
+      <c r="V53" s="78"/>
       <c r="W53" s="19"/>
       <c r="X53" s="19"/>
       <c r="Y53" s="19"/>
-      <c r="Z53" s="132"/>
-      <c r="AA53" s="133"/>
-      <c r="AB53" s="125"/>
+      <c r="Z53" s="135"/>
+      <c r="AA53" s="136"/>
+      <c r="AB53" s="87"/>
       <c r="AC53" s="63"/>
       <c r="AD53" s="63"/>
     </row>
-    <row r="54" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B54" s="106"/>
-      <c r="C54" s="114"/>
-      <c r="D54" s="111"/>
+    <row r="54" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="108"/>
+      <c r="C54" s="99"/>
+      <c r="D54" s="96"/>
       <c r="E54" s="18" t="s">
         <v>88</v>
       </c>
@@ -3930,21 +3941,21 @@
       <c r="P54" s="19"/>
       <c r="Q54" s="47"/>
       <c r="R54" s="47"/>
-      <c r="V54" s="50"/>
-      <c r="W54" s="19"/>
+      <c r="V54" s="78"/>
+      <c r="W54" s="78"/>
       <c r="X54" s="19"/>
       <c r="Y54" s="19"/>
-      <c r="Z54" s="132"/>
-      <c r="AA54" s="133"/>
-      <c r="AB54" s="125"/>
+      <c r="Z54" s="135"/>
+      <c r="AA54" s="136"/>
+      <c r="AB54" s="87"/>
       <c r="AC54" s="63"/>
       <c r="AD54" s="63"/>
     </row>
-    <row r="55" spans="1:30" s="6" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:30" s="6" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
-      <c r="B55" s="106"/>
-      <c r="C55" s="115"/>
-      <c r="D55" s="112"/>
+      <c r="B55" s="108"/>
+      <c r="C55" s="100"/>
+      <c r="D55" s="97"/>
       <c r="E55" s="22" t="s">
         <v>89</v>
       </c>
@@ -3967,26 +3978,26 @@
       <c r="P55" s="23"/>
       <c r="Q55" s="48"/>
       <c r="R55" s="48"/>
-      <c r="V55" s="52"/>
-      <c r="W55" s="23"/>
+      <c r="V55" s="78"/>
+      <c r="W55" s="79"/>
       <c r="X55" s="23"/>
       <c r="Y55" s="23"/>
-      <c r="Z55" s="132"/>
-      <c r="AA55" s="133"/>
-      <c r="AB55" s="125"/>
+      <c r="Z55" s="135"/>
+      <c r="AA55" s="136"/>
+      <c r="AB55" s="87"/>
       <c r="AC55" s="65"/>
       <c r="AD55" s="65"/>
     </row>
-    <row r="56" spans="1:30" s="10" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:30" s="10" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
-      <c r="B56" s="106"/>
-      <c r="C56" s="113" t="s">
+      <c r="B56" s="108"/>
+      <c r="C56" s="98" t="s">
         <v>90</v>
       </c>
-      <c r="D56" s="129" t="s">
+      <c r="D56" s="91" t="s">
         <v>92</v>
       </c>
-      <c r="E56" s="129"/>
+      <c r="E56" s="91"/>
       <c r="F56" s="19" t="s">
         <v>14</v>
       </c>
@@ -4010,19 +4021,19 @@
       <c r="T56" s="15"/>
       <c r="U56" s="15"/>
       <c r="V56" s="15"/>
-      <c r="W56" s="51"/>
-      <c r="X56" s="51"/>
-      <c r="Y56" s="15"/>
-      <c r="Z56" s="132"/>
-      <c r="AA56" s="133"/>
-      <c r="AB56" s="125"/>
+      <c r="W56" s="50"/>
+      <c r="X56" s="15"/>
+      <c r="Y56" s="139"/>
+      <c r="Z56" s="78"/>
+      <c r="AA56" s="78"/>
+      <c r="AB56" s="87"/>
       <c r="AC56" s="67"/>
       <c r="AD56" s="67"/>
     </row>
-    <row r="57" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B57" s="106"/>
-      <c r="C57" s="114"/>
-      <c r="D57" s="111" t="s">
+    <row r="57" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="108"/>
+      <c r="C57" s="99"/>
+      <c r="D57" s="96" t="s">
         <v>93</v>
       </c>
       <c r="E57" s="18" t="s">
@@ -4052,18 +4063,18 @@
       <c r="U57" s="19"/>
       <c r="V57" s="19"/>
       <c r="W57" s="50"/>
-      <c r="X57" s="50"/>
-      <c r="Y57" s="19"/>
-      <c r="Z57" s="132"/>
-      <c r="AA57" s="133"/>
-      <c r="AB57" s="125"/>
+      <c r="X57" s="19"/>
+      <c r="Y57" s="140"/>
+      <c r="Z57" s="78"/>
+      <c r="AA57" s="78"/>
+      <c r="AB57" s="87"/>
       <c r="AC57" s="63"/>
       <c r="AD57" s="63"/>
     </row>
-    <row r="58" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="106"/>
-      <c r="C58" s="114"/>
-      <c r="D58" s="111"/>
+    <row r="58" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="108"/>
+      <c r="C58" s="99"/>
+      <c r="D58" s="96"/>
       <c r="E58" s="18" t="s">
         <v>95</v>
       </c>
@@ -4092,17 +4103,17 @@
       <c r="V58" s="19"/>
       <c r="W58" s="50"/>
       <c r="X58" s="50"/>
-      <c r="Y58" s="19"/>
-      <c r="Z58" s="132"/>
-      <c r="AA58" s="133"/>
-      <c r="AB58" s="125"/>
+      <c r="Y58" s="32"/>
+      <c r="Z58" s="78"/>
+      <c r="AA58" s="136"/>
+      <c r="AB58" s="87"/>
       <c r="AC58" s="63"/>
       <c r="AD58" s="63"/>
     </row>
-    <row r="59" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B59" s="106"/>
-      <c r="C59" s="114"/>
-      <c r="D59" s="111"/>
+    <row r="59" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="108"/>
+      <c r="C59" s="99"/>
+      <c r="D59" s="96"/>
       <c r="E59" s="18" t="s">
         <v>96</v>
       </c>
@@ -4132,16 +4143,16 @@
       <c r="W59" s="50"/>
       <c r="X59" s="50"/>
       <c r="Y59" s="19"/>
-      <c r="Z59" s="132"/>
-      <c r="AA59" s="133"/>
-      <c r="AB59" s="125"/>
+      <c r="Z59" s="135"/>
+      <c r="AA59" s="78"/>
+      <c r="AB59" s="87"/>
       <c r="AC59" s="63"/>
       <c r="AD59" s="63"/>
     </row>
-    <row r="60" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B60" s="106"/>
-      <c r="C60" s="114"/>
-      <c r="D60" s="111"/>
+    <row r="60" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="108"/>
+      <c r="C60" s="99"/>
+      <c r="D60" s="96"/>
       <c r="E60" s="18" t="s">
         <v>97</v>
       </c>
@@ -4171,16 +4182,16 @@
       <c r="W60" s="50"/>
       <c r="X60" s="50"/>
       <c r="Y60" s="19"/>
-      <c r="Z60" s="132"/>
-      <c r="AA60" s="133"/>
-      <c r="AB60" s="125"/>
+      <c r="Z60" s="135"/>
+      <c r="AA60" s="78"/>
+      <c r="AB60" s="87"/>
       <c r="AC60" s="63"/>
       <c r="AD60" s="63"/>
     </row>
-    <row r="61" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B61" s="106"/>
-      <c r="C61" s="114"/>
-      <c r="D61" s="111" t="s">
+    <row r="61" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="108"/>
+      <c r="C61" s="99"/>
+      <c r="D61" s="96" t="s">
         <v>98</v>
       </c>
       <c r="E61" s="18" t="s">
@@ -4210,16 +4221,16 @@
       <c r="W61" s="19"/>
       <c r="X61" s="19"/>
       <c r="Y61" s="19"/>
-      <c r="Z61" s="132"/>
-      <c r="AA61" s="133"/>
-      <c r="AB61" s="125"/>
+      <c r="Z61" s="135"/>
+      <c r="AA61" s="136"/>
+      <c r="AB61" s="87"/>
       <c r="AC61" s="63"/>
       <c r="AD61" s="63"/>
     </row>
-    <row r="62" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B62" s="106"/>
-      <c r="C62" s="114"/>
-      <c r="D62" s="111"/>
+    <row r="62" spans="1:30" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="108"/>
+      <c r="C62" s="99"/>
+      <c r="D62" s="96"/>
       <c r="E62" s="18" t="s">
         <v>100</v>
       </c>
@@ -4247,17 +4258,17 @@
       <c r="W62" s="19"/>
       <c r="X62" s="19"/>
       <c r="Y62" s="19"/>
-      <c r="Z62" s="132"/>
-      <c r="AA62" s="133"/>
-      <c r="AB62" s="125"/>
+      <c r="Z62" s="135"/>
+      <c r="AA62" s="136"/>
+      <c r="AB62" s="87"/>
       <c r="AC62" s="63"/>
       <c r="AD62" s="63"/>
     </row>
-    <row r="63" spans="1:30" s="6" customFormat="1" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:30" s="6" customFormat="1" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
-      <c r="B63" s="106"/>
-      <c r="C63" s="115"/>
-      <c r="D63" s="112"/>
+      <c r="B63" s="108"/>
+      <c r="C63" s="100"/>
+      <c r="D63" s="97"/>
       <c r="E63" s="22" t="s">
         <v>101</v>
       </c>
@@ -4285,22 +4296,22 @@
       <c r="W63" s="23"/>
       <c r="X63" s="23"/>
       <c r="Y63" s="23"/>
-      <c r="Z63" s="132"/>
-      <c r="AA63" s="133"/>
-      <c r="AB63" s="125"/>
+      <c r="Z63" s="135"/>
+      <c r="AA63" s="136"/>
+      <c r="AB63" s="87"/>
       <c r="AC63" s="65"/>
       <c r="AD63" s="65"/>
     </row>
-    <row r="64" spans="1:30" s="10" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:30" s="10" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
-      <c r="B64" s="106"/>
-      <c r="C64" s="113" t="s">
+      <c r="B64" s="108"/>
+      <c r="C64" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="D64" s="129" t="s">
+      <c r="D64" s="91" t="s">
         <v>103</v>
       </c>
-      <c r="E64" s="129"/>
+      <c r="E64" s="91"/>
       <c r="F64" s="15" t="s">
         <v>14</v>
       </c>
@@ -4327,16 +4338,16 @@
       <c r="W64" s="15"/>
       <c r="X64" s="51"/>
       <c r="Y64" s="15"/>
-      <c r="Z64" s="132"/>
-      <c r="AA64" s="133"/>
-      <c r="AB64" s="125"/>
+      <c r="Z64" s="135"/>
+      <c r="AA64" s="78"/>
+      <c r="AB64" s="87"/>
       <c r="AC64" s="67"/>
       <c r="AD64" s="67"/>
     </row>
-    <row r="65" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B65" s="106"/>
-      <c r="C65" s="114"/>
-      <c r="D65" s="111" t="s">
+    <row r="65" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="108"/>
+      <c r="C65" s="99"/>
+      <c r="D65" s="96" t="s">
         <v>104</v>
       </c>
       <c r="E65" s="18" t="s">
@@ -4368,16 +4379,16 @@
       <c r="W65" s="19"/>
       <c r="X65" s="50"/>
       <c r="Y65" s="19"/>
-      <c r="Z65" s="132"/>
-      <c r="AA65" s="133"/>
-      <c r="AB65" s="125"/>
+      <c r="Z65" s="135"/>
+      <c r="AA65" s="78"/>
+      <c r="AB65" s="87"/>
       <c r="AC65" s="63"/>
       <c r="AD65" s="63"/>
     </row>
-    <row r="66" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B66" s="106"/>
-      <c r="C66" s="114"/>
-      <c r="D66" s="111"/>
+    <row r="66" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="108"/>
+      <c r="C66" s="99"/>
+      <c r="D66" s="96"/>
       <c r="E66" s="18" t="s">
         <v>106</v>
       </c>
@@ -4407,16 +4418,16 @@
       <c r="W66" s="19"/>
       <c r="X66" s="50"/>
       <c r="Y66" s="19"/>
-      <c r="Z66" s="132"/>
-      <c r="AA66" s="133"/>
-      <c r="AB66" s="125"/>
+      <c r="Z66" s="135"/>
+      <c r="AA66" s="78"/>
+      <c r="AB66" s="87"/>
       <c r="AC66" s="63"/>
       <c r="AD66" s="63"/>
     </row>
-    <row r="67" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B67" s="106"/>
-      <c r="C67" s="114"/>
-      <c r="D67" s="111"/>
+    <row r="67" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="108"/>
+      <c r="C67" s="99"/>
+      <c r="D67" s="96"/>
       <c r="E67" s="18" t="s">
         <v>107</v>
       </c>
@@ -4446,16 +4457,16 @@
       <c r="W67" s="19"/>
       <c r="X67" s="50"/>
       <c r="Y67" s="19"/>
-      <c r="Z67" s="132"/>
-      <c r="AA67" s="133"/>
-      <c r="AB67" s="125"/>
+      <c r="Z67" s="135"/>
+      <c r="AA67" s="78"/>
+      <c r="AB67" s="87"/>
       <c r="AC67" s="63"/>
       <c r="AD67" s="63"/>
     </row>
-    <row r="68" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B68" s="106"/>
-      <c r="C68" s="114"/>
-      <c r="D68" s="111"/>
+    <row r="68" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="108"/>
+      <c r="C68" s="99"/>
+      <c r="D68" s="96"/>
       <c r="E68" s="18" t="s">
         <v>108</v>
       </c>
@@ -4485,16 +4496,16 @@
       <c r="W68" s="19"/>
       <c r="X68" s="50"/>
       <c r="Y68" s="19"/>
-      <c r="Z68" s="132"/>
-      <c r="AA68" s="133"/>
-      <c r="AB68" s="125"/>
+      <c r="Z68" s="135"/>
+      <c r="AA68" s="78"/>
+      <c r="AB68" s="87"/>
       <c r="AC68" s="63"/>
       <c r="AD68" s="63"/>
     </row>
-    <row r="69" spans="1:30" s="6" customFormat="1" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:30" s="6" customFormat="1" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
-      <c r="B69" s="106"/>
-      <c r="C69" s="115"/>
+      <c r="B69" s="108"/>
+      <c r="C69" s="100"/>
       <c r="D69" s="22" t="s">
         <v>109</v>
       </c>
@@ -4525,21 +4536,21 @@
       <c r="W69" s="23"/>
       <c r="X69" s="23"/>
       <c r="Y69" s="23"/>
-      <c r="Z69" s="132"/>
-      <c r="AA69" s="133"/>
-      <c r="AB69" s="125"/>
+      <c r="Z69" s="135"/>
+      <c r="AA69" s="136"/>
+      <c r="AB69" s="87"/>
       <c r="AC69" s="65"/>
       <c r="AD69" s="65"/>
     </row>
-    <row r="70" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B70" s="106"/>
-      <c r="C70" s="113" t="s">
+    <row r="70" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="108"/>
+      <c r="C70" s="98" t="s">
         <v>147</v>
       </c>
-      <c r="D70" s="128" t="s">
+      <c r="D70" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="E70" s="128"/>
+      <c r="E70" s="90"/>
       <c r="F70" s="15" t="s">
         <v>14</v>
       </c>
@@ -4566,16 +4577,16 @@
       <c r="W70" s="15"/>
       <c r="X70" s="15"/>
       <c r="Y70" s="74"/>
-      <c r="Z70" s="132"/>
-      <c r="AA70" s="133"/>
-      <c r="AB70" s="125"/>
+      <c r="Z70" s="135"/>
+      <c r="AA70" s="136"/>
+      <c r="AB70" s="87"/>
       <c r="AC70" s="63"/>
       <c r="AD70" s="63"/>
     </row>
-    <row r="71" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B71" s="106"/>
-      <c r="C71" s="114"/>
-      <c r="D71" s="111" t="s">
+    <row r="71" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="108"/>
+      <c r="C71" s="99"/>
+      <c r="D71" s="96" t="s">
         <v>112</v>
       </c>
       <c r="E71" s="18" t="s">
@@ -4607,16 +4618,16 @@
       <c r="W71" s="19"/>
       <c r="X71" s="19"/>
       <c r="Y71" s="75"/>
-      <c r="Z71" s="132"/>
-      <c r="AA71" s="133"/>
-      <c r="AB71" s="125"/>
+      <c r="Z71" s="135"/>
+      <c r="AA71" s="136"/>
+      <c r="AB71" s="87"/>
       <c r="AC71" s="63"/>
       <c r="AD71" s="63"/>
     </row>
-    <row r="72" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B72" s="106"/>
-      <c r="C72" s="114"/>
-      <c r="D72" s="111"/>
+    <row r="72" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="108"/>
+      <c r="C72" s="99"/>
+      <c r="D72" s="96"/>
       <c r="E72" s="18" t="s">
         <v>114</v>
       </c>
@@ -4646,16 +4657,16 @@
       <c r="W72" s="19"/>
       <c r="X72" s="19"/>
       <c r="Y72" s="75"/>
-      <c r="Z72" s="132"/>
-      <c r="AA72" s="133"/>
-      <c r="AB72" s="125"/>
+      <c r="Z72" s="135"/>
+      <c r="AA72" s="136"/>
+      <c r="AB72" s="87"/>
       <c r="AC72" s="63"/>
       <c r="AD72" s="63"/>
     </row>
-    <row r="73" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B73" s="106"/>
-      <c r="C73" s="114"/>
-      <c r="D73" s="111"/>
+    <row r="73" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="108"/>
+      <c r="C73" s="99"/>
+      <c r="D73" s="96"/>
       <c r="E73" s="18" t="s">
         <v>115</v>
       </c>
@@ -4685,16 +4696,16 @@
       <c r="W73" s="19"/>
       <c r="X73" s="19"/>
       <c r="Y73" s="75"/>
-      <c r="Z73" s="132"/>
-      <c r="AA73" s="133"/>
-      <c r="AB73" s="125"/>
+      <c r="Z73" s="135"/>
+      <c r="AA73" s="136"/>
+      <c r="AB73" s="87"/>
       <c r="AC73" s="63"/>
       <c r="AD73" s="63"/>
     </row>
-    <row r="74" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B74" s="106"/>
-      <c r="C74" s="114"/>
-      <c r="D74" s="111" t="s">
+    <row r="74" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="108"/>
+      <c r="C74" s="99"/>
+      <c r="D74" s="96" t="s">
         <v>116</v>
       </c>
       <c r="E74" s="18" t="s">
@@ -4726,16 +4737,16 @@
       <c r="W74" s="19"/>
       <c r="X74" s="19"/>
       <c r="Y74" s="75"/>
-      <c r="Z74" s="132"/>
-      <c r="AA74" s="133"/>
-      <c r="AB74" s="125"/>
+      <c r="Z74" s="135"/>
+      <c r="AA74" s="136"/>
+      <c r="AB74" s="87"/>
       <c r="AC74" s="63"/>
       <c r="AD74" s="63"/>
     </row>
-    <row r="75" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B75" s="106"/>
-      <c r="C75" s="114"/>
-      <c r="D75" s="111"/>
+    <row r="75" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="108"/>
+      <c r="C75" s="99"/>
+      <c r="D75" s="96"/>
       <c r="E75" s="18" t="s">
         <v>118</v>
       </c>
@@ -4765,16 +4776,16 @@
       <c r="W75" s="19"/>
       <c r="X75" s="19"/>
       <c r="Y75" s="75"/>
-      <c r="Z75" s="132"/>
-      <c r="AA75" s="133"/>
-      <c r="AB75" s="125"/>
+      <c r="Z75" s="135"/>
+      <c r="AA75" s="136"/>
+      <c r="AB75" s="87"/>
       <c r="AC75" s="63"/>
       <c r="AD75" s="63"/>
     </row>
-    <row r="76" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B76" s="106"/>
-      <c r="C76" s="114"/>
-      <c r="D76" s="111"/>
+    <row r="76" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="108"/>
+      <c r="C76" s="99"/>
+      <c r="D76" s="96"/>
       <c r="E76" s="18" t="s">
         <v>119</v>
       </c>
@@ -4804,17 +4815,17 @@
       <c r="W76" s="19"/>
       <c r="X76" s="19"/>
       <c r="Y76" s="75"/>
-      <c r="Z76" s="132"/>
-      <c r="AA76" s="133"/>
-      <c r="AB76" s="125"/>
+      <c r="Z76" s="135"/>
+      <c r="AA76" s="136"/>
+      <c r="AB76" s="87"/>
       <c r="AC76" s="63"/>
       <c r="AD76" s="63"/>
     </row>
-    <row r="77" spans="1:30" s="6" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:30" s="6" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
-      <c r="B77" s="107"/>
-      <c r="C77" s="115"/>
-      <c r="D77" s="112"/>
+      <c r="B77" s="109"/>
+      <c r="C77" s="100"/>
+      <c r="D77" s="97"/>
       <c r="E77" s="22" t="s">
         <v>120</v>
       </c>
@@ -4844,44 +4855,36 @@
       <c r="W77" s="23"/>
       <c r="X77" s="23"/>
       <c r="Y77" s="76"/>
-      <c r="Z77" s="134"/>
-      <c r="AA77" s="135"/>
-      <c r="AB77" s="126"/>
+      <c r="Z77" s="137"/>
+      <c r="AA77" s="138"/>
+      <c r="AB77" s="88"/>
       <c r="AC77" s="65"/>
       <c r="AD77" s="65"/>
     </row>
-    <row r="78" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G78" s="9"/>
     </row>
-    <row r="79" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="80" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="81" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="82" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="83" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="84" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="79" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="AB9:AB77"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="Z32:AA77"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="C64:C69"/>
-    <mergeCell ref="D65:D68"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="D74:D77"/>
-    <mergeCell ref="C70:C77"/>
-    <mergeCell ref="C12:C20"/>
-    <mergeCell ref="B9:B22"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="D12:D20"/>
+    <mergeCell ref="X7:AD7"/>
+    <mergeCell ref="N2:AB4"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="J6:W6"/>
+    <mergeCell ref="X6:AD6"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="J7:P7"/>
+    <mergeCell ref="Q7:W7"/>
     <mergeCell ref="B32:B77"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="D61:D63"/>
@@ -4898,19 +4901,27 @@
     <mergeCell ref="D36:D38"/>
     <mergeCell ref="D43:D44"/>
     <mergeCell ref="C9:C11"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="J7:P7"/>
-    <mergeCell ref="Q7:W7"/>
-    <mergeCell ref="X7:AD7"/>
-    <mergeCell ref="N2:AB4"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="J6:W6"/>
-    <mergeCell ref="X6:AD6"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="C12:C20"/>
+    <mergeCell ref="B9:B22"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="D12:D20"/>
+    <mergeCell ref="C64:C69"/>
+    <mergeCell ref="D65:D68"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="D74:D77"/>
+    <mergeCell ref="C70:C77"/>
+    <mergeCell ref="AB9:AB77"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="Z32:AA35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>